<commit_message>
[INFRA] update QDA stats table
</commit_message>
<xml_diff>
--- a/Docs/Result Summary.xlsx
+++ b/Docs/Result Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i560646/Desktop/Eden/ML Final Project/Image_Based_Malware_Classification/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FA5DB9E-92C9-E242-8329-F52D2EEDBFCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AE64F7-4473-7B42-9A4D-3C1CB5D26090}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57600" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="21">
   <si>
     <t>LDA</t>
   </si>
@@ -204,20 +204,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -230,7 +218,16 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,1166 +546,1178 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF31505B-2C63-644B-873C-2CE4A29A5DA4}">
   <dimension ref="D2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="S13" sqref="S13"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="5"/>
-    <col min="4" max="4" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="5"/>
-    <col min="10" max="10" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="5"/>
-    <col min="16" max="16" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.83203125" style="5"/>
-    <col min="19" max="19" width="11.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="5" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="13" style="5" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="5"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="1"/>
+    <col min="16" max="16" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.83203125" style="1"/>
+    <col min="19" max="19" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="3"/>
-      <c r="R2" s="4" t="s">
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="7"/>
+      <c r="R2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="4"/>
-      <c r="T2" s="4"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
     </row>
     <row r="3" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H3" s="7" t="s">
+      <c r="G3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="7" t="s">
+      <c r="R3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="7" t="s">
+      <c r="S3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="7" t="s">
+      <c r="T3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="7" t="s">
+      <c r="U3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="7" t="s">
+      <c r="V3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="2">
         <v>8</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="2">
         <v>96.968999999999994</v>
       </c>
-      <c r="G4" s="6">
+      <c r="G4" s="2">
         <v>98.373000000000005</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="2">
         <v>98.198999999999998</v>
       </c>
-      <c r="R4" s="8" t="s">
+      <c r="R4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="2">
         <v>6</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="2">
         <v>97.009</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="2">
         <v>2</v>
       </c>
-      <c r="V4" s="6">
+      <c r="V4" s="2">
         <v>99.15</v>
       </c>
     </row>
     <row r="5" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E5" s="6">
-        <v>10</v>
-      </c>
-      <c r="F5" s="6">
+      <c r="E5" s="2">
+        <v>10</v>
+      </c>
+      <c r="F5" s="2">
         <v>97.346999999999994</v>
       </c>
-      <c r="G5" s="6">
+      <c r="G5" s="2">
         <v>99.933000000000007</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="2">
         <v>99.674000000000007</v>
       </c>
-      <c r="R5" s="8" t="s">
+      <c r="R5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S5" s="6">
-        <v>10</v>
-      </c>
-      <c r="T5" s="6">
+      <c r="S5" s="2">
+        <v>10</v>
+      </c>
+      <c r="T5" s="2">
         <v>97.346999999999994</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="2">
         <v>2</v>
       </c>
-      <c r="V5" s="6">
+      <c r="V5" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="6" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="6">
-        <v>10</v>
-      </c>
-      <c r="F6" s="6">
+      <c r="D6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="2">
+        <v>10</v>
+      </c>
+      <c r="F6" s="2">
         <v>65.015000000000001</v>
       </c>
-      <c r="G6" s="6">
-        <v>100</v>
-      </c>
-      <c r="H6" s="6">
+      <c r="G6" s="2">
+        <v>100</v>
+      </c>
+      <c r="H6" s="2">
         <v>96.501000000000005</v>
       </c>
-      <c r="R6" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S6" s="6">
-        <v>3</v>
-      </c>
-      <c r="T6" s="6">
+      <c r="R6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S6" s="2">
+        <v>3</v>
+      </c>
+      <c r="T6" s="2">
         <v>70.73</v>
       </c>
-      <c r="U6" s="6" t="s">
+      <c r="U6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V6" s="6">
+      <c r="V6" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="9" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="3"/>
-      <c r="R9" s="4" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="7"/>
+      <c r="R9" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
+      <c r="S9" s="8"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
     </row>
     <row r="10" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="7" t="s">
+      <c r="G10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S10" s="7" t="s">
+      <c r="S10" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T10" s="7" t="s">
+      <c r="T10" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U10" s="7" t="s">
+      <c r="U10" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V10" s="7" t="s">
+      <c r="V10" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="11" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="2">
         <v>6</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F11" s="2">
         <v>95.238</v>
       </c>
-      <c r="G11" s="6">
+      <c r="G11" s="2">
         <v>95.459000000000003</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="2">
         <v>95.421999999999997</v>
       </c>
-      <c r="R11" s="8" t="s">
+      <c r="R11" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="2">
         <v>9</v>
       </c>
-      <c r="T11" s="6">
+      <c r="T11" s="2">
         <v>95.257999999999996</v>
       </c>
-      <c r="U11" s="6">
+      <c r="U11" s="2">
         <v>2</v>
       </c>
-      <c r="V11" s="6">
+      <c r="V11" s="2">
         <v>95.677999999999997</v>
       </c>
     </row>
     <row r="12" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D12" s="8" t="s">
+      <c r="D12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="6">
-        <v>3</v>
-      </c>
-      <c r="F12" s="6">
+      <c r="E12" s="2">
+        <v>3</v>
+      </c>
+      <c r="F12" s="2">
         <v>96.466999999999999</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="2">
         <v>96.881</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="2">
         <v>96.742999999999995</v>
       </c>
-      <c r="R12" s="8" t="s">
+      <c r="R12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S12" s="6">
-        <v>3</v>
-      </c>
-      <c r="T12" s="6">
+      <c r="S12" s="2">
+        <v>3</v>
+      </c>
+      <c r="T12" s="2">
         <v>96.466999999999999</v>
       </c>
-      <c r="U12" s="6">
+      <c r="U12" s="2">
         <v>2</v>
       </c>
-      <c r="V12" s="6">
+      <c r="V12" s="2">
         <v>97.111000000000004</v>
       </c>
     </row>
     <row r="13" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="6">
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="2">
         <v>9</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>96.885999999999996</v>
       </c>
-      <c r="G13" s="6">
+      <c r="G13" s="2">
         <v>97.299000000000007</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="2">
         <v>97.253</v>
       </c>
-      <c r="R13" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S13" s="6">
-        <v>3</v>
-      </c>
-      <c r="T13" s="6">
+      <c r="R13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S13" s="2">
+        <v>3</v>
+      </c>
+      <c r="T13" s="2">
         <v>96.887</v>
       </c>
-      <c r="U13" s="6">
+      <c r="U13" s="2">
         <v>2</v>
       </c>
-      <c r="V13" s="6">
+      <c r="V13" s="2">
         <v>97.634</v>
       </c>
     </row>
     <row r="16" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D16" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="3"/>
-      <c r="R16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="4"/>
-      <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
+      <c r="D16" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+      <c r="R16" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="S16" s="8"/>
+      <c r="T16" s="8"/>
+      <c r="U16" s="8"/>
+      <c r="V16" s="8"/>
     </row>
     <row r="17" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="7" t="s">
+      <c r="F17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="7" t="s">
+      <c r="G17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R17" s="7" t="s">
+      <c r="R17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S17" s="7" t="s">
+      <c r="S17" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T17" s="7" t="s">
+      <c r="T17" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U17" s="7" t="s">
+      <c r="U17" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V17" s="7" t="s">
+      <c r="V17" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D18" s="8" t="s">
+      <c r="D18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="6">
-        <v>10</v>
-      </c>
-      <c r="F18" s="5">
+      <c r="E18" s="2">
+        <v>10</v>
+      </c>
+      <c r="F18" s="1">
         <v>58.223999999999997</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="2">
         <v>93.820999999999998</v>
       </c>
-      <c r="H18" s="6">
+      <c r="H18" s="2">
         <v>90.260999999999996</v>
       </c>
-      <c r="R18" s="8" t="s">
+      <c r="R18" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S18" s="6">
-        <v>10</v>
-      </c>
-      <c r="T18" s="6">
+      <c r="S18" s="2">
+        <v>10</v>
+      </c>
+      <c r="T18" s="2">
         <v>58.223999999999997</v>
       </c>
-      <c r="U18" s="6">
+      <c r="U18" s="2">
         <v>2</v>
       </c>
-      <c r="V18" s="6">
+      <c r="V18" s="2">
         <v>96.814999999999998</v>
       </c>
     </row>
     <row r="19" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D19" s="8" t="s">
+      <c r="D19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="6">
-        <v>10</v>
-      </c>
-      <c r="F19" s="6">
+      <c r="E19" s="2">
+        <v>10</v>
+      </c>
+      <c r="F19" s="2">
         <v>50.307000000000002</v>
       </c>
-      <c r="G19" s="6">
-        <v>100</v>
-      </c>
-      <c r="H19" s="6">
+      <c r="G19" s="2">
+        <v>100</v>
+      </c>
+      <c r="H19" s="2">
         <v>95.031000000000006</v>
       </c>
-      <c r="R19" s="8" t="s">
+      <c r="R19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S19" s="6">
+      <c r="S19" s="2">
         <v>4</v>
       </c>
-      <c r="T19" s="6">
+      <c r="T19" s="2">
         <v>54.914999999999999</v>
       </c>
-      <c r="U19" s="6" t="s">
+      <c r="U19" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V19" s="6">
+      <c r="V19" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="20" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="R20" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S20" s="6"/>
-      <c r="T20" s="6"/>
-      <c r="U20" s="6"/>
-      <c r="V20" s="6"/>
+      <c r="D20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E20" s="2">
+        <v>10</v>
+      </c>
+      <c r="F20" s="2">
+        <v>48.884</v>
+      </c>
+      <c r="G20" s="2">
+        <v>100</v>
+      </c>
+      <c r="H20" s="2">
+        <v>94.888000000000005</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S20" s="2">
+        <v>7</v>
+      </c>
+      <c r="T20" s="2">
+        <v>48.975999999999999</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V20" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D23" s="1" t="s">
+      <c r="D23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="3"/>
-      <c r="J23" s="1" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="7"/>
+      <c r="J23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="3"/>
-      <c r="R23" s="1" t="s">
+      <c r="K23" s="6"/>
+      <c r="L23" s="6"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="7"/>
+      <c r="R23" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="S23" s="2"/>
-      <c r="T23" s="2"/>
-      <c r="U23" s="2"/>
-      <c r="V23" s="3"/>
-      <c r="X23" s="4" t="s">
+      <c r="S23" s="6"/>
+      <c r="T23" s="6"/>
+      <c r="U23" s="6"/>
+      <c r="V23" s="7"/>
+      <c r="X23" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="4"/>
-      <c r="Z23" s="4"/>
-      <c r="AA23" s="4"/>
-      <c r="AB23" s="4"/>
+      <c r="Y23" s="8"/>
+      <c r="Z23" s="8"/>
+      <c r="AA23" s="8"/>
+      <c r="AB23" s="8"/>
     </row>
     <row r="24" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="7" t="s">
+      <c r="E24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H24" s="7" t="s">
+      <c r="G24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="7" t="s">
+      <c r="J24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="7" t="s">
+      <c r="K24" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="7" t="s">
+      <c r="L24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N24" s="7" t="s">
+      <c r="M24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R24" s="7" t="s">
+      <c r="R24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S24" s="7" t="s">
+      <c r="S24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T24" s="7" t="s">
+      <c r="T24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U24" s="7" t="s">
+      <c r="U24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V24" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="X24" s="7" t="s">
+      <c r="V24" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X24" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Y24" s="7" t="s">
+      <c r="Y24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Z24" s="7" t="s">
+      <c r="Z24" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA24" s="7" t="s">
+      <c r="AA24" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB24" s="7" t="s">
+      <c r="AB24" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="25" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D25" s="8" t="s">
+      <c r="D25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="6">
+      <c r="E25" s="2">
         <v>8</v>
       </c>
-      <c r="F25" s="6">
+      <c r="F25" s="2">
         <v>98.71</v>
       </c>
-      <c r="G25" s="6">
+      <c r="G25" s="2">
         <v>99.188000000000002</v>
       </c>
-      <c r="H25" s="6">
+      <c r="H25" s="2">
         <v>99.128</v>
       </c>
-      <c r="J25" s="8" t="s">
+      <c r="J25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K25" s="6">
-        <v>10</v>
-      </c>
-      <c r="L25" s="6">
+      <c r="K25" s="2">
+        <v>10</v>
+      </c>
+      <c r="L25" s="2">
         <v>99.15</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M25" s="2">
         <v>99.465999999999994</v>
       </c>
-      <c r="N25" s="6">
+      <c r="N25" s="2">
         <v>99.435000000000002</v>
       </c>
-      <c r="R25" s="8" t="s">
+      <c r="R25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S25" s="6">
+      <c r="S25" s="2">
         <v>8</v>
       </c>
-      <c r="T25" s="6">
+      <c r="T25" s="2">
         <v>98.71</v>
       </c>
-      <c r="U25" s="6">
+      <c r="U25" s="2">
         <v>8</v>
       </c>
-      <c r="V25" s="6">
+      <c r="V25" s="2">
         <v>99.188000000000002</v>
       </c>
-      <c r="X25" s="8" t="s">
+      <c r="X25" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Y25" s="6">
-        <v>10</v>
-      </c>
-      <c r="Z25" s="6">
+      <c r="Y25" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z25" s="2">
         <v>99.15</v>
       </c>
-      <c r="AA25" s="9">
-        <v>10</v>
-      </c>
-      <c r="AB25" s="6">
+      <c r="AA25" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB25" s="2">
         <v>99.465999999999994</v>
       </c>
     </row>
     <row r="26" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D26" s="8" t="s">
+      <c r="D26" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E26" s="6">
+      <c r="E26" s="2">
         <v>8</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="2">
         <v>99.754000000000005</v>
       </c>
-      <c r="G26" s="6">
+      <c r="G26" s="2">
         <v>99.997</v>
       </c>
-      <c r="H26" s="6">
+      <c r="H26" s="2">
         <v>99.966999999999999</v>
       </c>
-      <c r="J26" s="8" t="s">
+      <c r="J26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K26" s="6">
-        <v>10</v>
-      </c>
-      <c r="L26" s="6">
+      <c r="K26" s="2">
+        <v>10</v>
+      </c>
+      <c r="L26" s="2">
         <v>99.825999999999993</v>
       </c>
-      <c r="M26" s="6">
-        <v>100</v>
-      </c>
-      <c r="N26" s="6">
+      <c r="M26" s="2">
+        <v>100</v>
+      </c>
+      <c r="N26" s="2">
         <v>99.983000000000004</v>
       </c>
-      <c r="R26" s="8" t="s">
+      <c r="R26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S26" s="6">
+      <c r="S26" s="2">
         <v>8</v>
       </c>
-      <c r="T26" s="6">
+      <c r="T26" s="2">
         <v>99.754000000000005</v>
       </c>
-      <c r="U26" s="5">
+      <c r="U26" s="1">
         <v>8</v>
       </c>
-      <c r="V26" s="6">
+      <c r="V26" s="2">
         <v>99.997</v>
       </c>
-      <c r="X26" s="8" t="s">
+      <c r="X26" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Y26" s="6">
-        <v>10</v>
-      </c>
-      <c r="Z26" s="6">
+      <c r="Y26" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z26" s="2">
         <v>99.825999999999993</v>
       </c>
-      <c r="AA26" s="9">
-        <v>10</v>
-      </c>
-      <c r="AB26" s="6">
+      <c r="AA26" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB26" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="27" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="6">
+      <c r="D27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="2">
         <v>9</v>
       </c>
-      <c r="F27" s="6">
+      <c r="F27" s="2">
         <v>99.816000000000003</v>
       </c>
-      <c r="G27" s="6">
-        <v>100</v>
-      </c>
-      <c r="H27" s="6">
+      <c r="G27" s="2">
+        <v>100</v>
+      </c>
+      <c r="H27" s="2">
         <v>99.981999999999999</v>
       </c>
-      <c r="J27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="6">
+      <c r="J27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K27" s="2">
         <v>8</v>
       </c>
-      <c r="L27" s="6">
+      <c r="L27" s="2">
         <v>99.775000000000006</v>
       </c>
-      <c r="M27" s="6">
-        <v>100</v>
-      </c>
-      <c r="N27" s="6">
+      <c r="M27" s="2">
+        <v>100</v>
+      </c>
+      <c r="N27" s="2">
         <v>99.974999999999994</v>
       </c>
-      <c r="R27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S27" s="6">
-        <v>10</v>
-      </c>
-      <c r="T27" s="6">
+      <c r="R27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S27" s="2">
+        <v>10</v>
+      </c>
+      <c r="T27" s="2">
         <v>99.816000000000003</v>
       </c>
-      <c r="U27" s="6">
-        <v>10</v>
-      </c>
-      <c r="V27" s="6">
-        <v>100</v>
-      </c>
-      <c r="X27" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y27" s="6">
+      <c r="U27" s="2">
+        <v>10</v>
+      </c>
+      <c r="V27" s="2">
+        <v>100</v>
+      </c>
+      <c r="X27" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y27" s="2">
         <v>9</v>
       </c>
-      <c r="Z27" s="6">
+      <c r="Z27" s="2">
         <v>99.775000000000006</v>
       </c>
-      <c r="AA27" s="6">
+      <c r="AA27" s="2">
         <v>9</v>
       </c>
-      <c r="AB27" s="6">
+      <c r="AB27" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="30" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D30" s="1" t="s">
+      <c r="D30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="3"/>
-      <c r="J30" s="1" t="s">
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
+      <c r="J30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
-      <c r="N30" s="3"/>
-      <c r="R30" s="1" t="s">
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="7"/>
+      <c r="R30" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="S30" s="2"/>
-      <c r="T30" s="2"/>
-      <c r="U30" s="2"/>
-      <c r="V30" s="3"/>
-      <c r="X30" s="1" t="s">
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="6"/>
+      <c r="V30" s="7"/>
+      <c r="X30" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="Y30" s="2"/>
-      <c r="Z30" s="2"/>
-      <c r="AA30" s="2"/>
-      <c r="AB30" s="3"/>
+      <c r="Y30" s="6"/>
+      <c r="Z30" s="6"/>
+      <c r="AA30" s="6"/>
+      <c r="AB30" s="7"/>
     </row>
     <row r="31" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D31" s="7" t="s">
+      <c r="D31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E31" s="7" t="s">
+      <c r="E31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="7" t="s">
+      <c r="F31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="7" t="s">
+      <c r="G31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J31" s="7" t="s">
+      <c r="J31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K31" s="7" t="s">
+      <c r="K31" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L31" s="7" t="s">
+      <c r="L31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="N31" s="7" t="s">
+      <c r="M31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R31" s="7" t="s">
+      <c r="R31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S31" s="7" t="s">
+      <c r="S31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T31" s="7" t="s">
+      <c r="T31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U31" s="7" t="s">
+      <c r="U31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V31" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="X31" s="7" t="s">
+      <c r="V31" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="X31" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="Y31" s="7" t="s">
+      <c r="Y31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="Z31" s="7" t="s">
+      <c r="Z31" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="AA31" s="7" t="s">
+      <c r="AA31" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="AB31" s="7" t="s">
+      <c r="AB31" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="32" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D32" s="8" t="s">
+      <c r="D32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E32" s="6">
-        <v>10</v>
-      </c>
-      <c r="F32" s="6">
+      <c r="E32" s="2">
+        <v>10</v>
+      </c>
+      <c r="F32" s="2">
         <v>99.385999999999996</v>
       </c>
-      <c r="G32" s="6">
+      <c r="G32" s="2">
         <v>99.701999999999998</v>
       </c>
-      <c r="H32" s="6">
+      <c r="H32" s="2">
         <v>99.67</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K32" s="6">
+      <c r="K32" s="2">
         <v>9</v>
       </c>
-      <c r="L32" s="6">
+      <c r="L32" s="2">
         <v>99.528999999999996</v>
       </c>
-      <c r="M32" s="6">
+      <c r="M32" s="2">
         <v>99.763999999999996</v>
       </c>
-      <c r="N32" s="6">
+      <c r="N32" s="2">
         <v>99.738</v>
       </c>
-      <c r="R32" s="8" t="s">
+      <c r="R32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S32" s="6">
-        <v>10</v>
-      </c>
-      <c r="T32" s="6">
+      <c r="S32" s="2">
+        <v>10</v>
+      </c>
+      <c r="T32" s="2">
         <v>99.385999999999996</v>
       </c>
-      <c r="U32" s="5">
-        <v>10</v>
-      </c>
-      <c r="V32" s="6">
+      <c r="U32" s="1">
+        <v>10</v>
+      </c>
+      <c r="V32" s="2">
         <v>99.701999999999998</v>
       </c>
-      <c r="X32" s="8" t="s">
+      <c r="X32" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="Y32" s="6">
+      <c r="Y32" s="2">
         <v>9</v>
       </c>
-      <c r="Z32" s="6">
+      <c r="Z32" s="2">
         <v>99.528999999999996</v>
       </c>
-      <c r="AA32" s="9">
+      <c r="AA32" s="2">
         <v>9</v>
       </c>
-      <c r="AB32" s="6">
+      <c r="AB32" s="2">
         <v>99.763999999999996</v>
       </c>
     </row>
     <row r="33" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E33" s="6">
-        <v>10</v>
-      </c>
-      <c r="F33" s="6">
+      <c r="E33" s="2">
+        <v>10</v>
+      </c>
+      <c r="F33" s="2">
         <v>99.703000000000003</v>
       </c>
-      <c r="G33" s="6">
-        <v>100</v>
-      </c>
-      <c r="H33" s="6">
+      <c r="G33" s="2">
+        <v>100</v>
+      </c>
+      <c r="H33" s="2">
         <v>99.97</v>
       </c>
-      <c r="J33" s="8" t="s">
+      <c r="J33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K33" s="6">
-        <v>10</v>
-      </c>
-      <c r="L33" s="6">
+      <c r="K33" s="2">
+        <v>10</v>
+      </c>
+      <c r="L33" s="2">
         <v>99.754000000000005</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="2">
         <v>99.997</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="2">
         <v>99.971999999999994</v>
       </c>
-      <c r="R33" s="8" t="s">
+      <c r="R33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S33" s="6">
+      <c r="S33" s="2">
         <v>9</v>
       </c>
-      <c r="T33" s="6">
+      <c r="T33" s="2">
         <v>99.724000000000004</v>
       </c>
-      <c r="U33" s="6">
+      <c r="U33" s="2">
         <v>9</v>
       </c>
-      <c r="V33" s="6">
-        <v>100</v>
-      </c>
-      <c r="X33" s="8" t="s">
+      <c r="V33" s="2">
+        <v>100</v>
+      </c>
+      <c r="X33" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="Y33" s="6">
-        <v>10</v>
-      </c>
-      <c r="Z33" s="6">
+      <c r="Y33" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z33" s="2">
         <v>99.754000000000005</v>
       </c>
-      <c r="AA33" s="6">
-        <v>10</v>
-      </c>
-      <c r="AB33" s="6">
+      <c r="AA33" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB33" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="34" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="6">
+      <c r="D34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E34" s="2">
         <v>9</v>
       </c>
-      <c r="F34" s="6">
+      <c r="F34" s="2">
         <v>99.775000000000006</v>
       </c>
-      <c r="G34" s="6">
-        <v>100</v>
-      </c>
-      <c r="H34" s="6">
+      <c r="G34" s="2">
+        <v>100</v>
+      </c>
+      <c r="H34" s="2">
         <v>99.977000000000004</v>
       </c>
-      <c r="J34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="K34" s="6">
+      <c r="J34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K34" s="2">
         <v>9</v>
       </c>
-      <c r="L34" s="6">
+      <c r="L34" s="2">
         <v>99.733999999999995</v>
       </c>
-      <c r="M34" s="6">
-        <v>100</v>
-      </c>
-      <c r="N34" s="6">
+      <c r="M34" s="2">
+        <v>100</v>
+      </c>
+      <c r="N34" s="2">
         <v>99.972999999999999</v>
       </c>
-      <c r="R34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S34" s="6">
-        <v>10</v>
-      </c>
-      <c r="T34" s="6">
+      <c r="R34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S34" s="2">
+        <v>10</v>
+      </c>
+      <c r="T34" s="2">
         <v>99.775000000000006</v>
       </c>
-      <c r="U34" s="6">
-        <v>10</v>
-      </c>
-      <c r="V34" s="6">
-        <v>100</v>
-      </c>
-      <c r="X34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y34" s="6">
-        <v>10</v>
-      </c>
-      <c r="Z34" s="6">
+      <c r="U34" s="2">
+        <v>10</v>
+      </c>
+      <c r="V34" s="2">
+        <v>100</v>
+      </c>
+      <c r="X34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z34" s="2">
         <v>99.733999999999995</v>
       </c>
-      <c r="AA34" s="6">
-        <v>10</v>
-      </c>
-      <c r="AB34" s="6">
+      <c r="AA34" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB34" s="2">
         <v>100</v>
       </c>
     </row>
     <row r="35" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="AA35" s="5" t="s">
+      <c r="AA35" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D37" s="1" t="s">
+      <c r="D37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
-      <c r="H37" s="3"/>
-      <c r="R37" s="1" t="s">
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="7"/>
+      <c r="R37" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="2"/>
-      <c r="T37" s="2"/>
-      <c r="U37" s="2"/>
-      <c r="V37" s="3"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+      <c r="U37" s="6"/>
+      <c r="V37" s="7"/>
     </row>
     <row r="38" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D38" s="7" t="s">
+      <c r="D38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="E38" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F38" s="7" t="s">
+      <c r="F38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="H38" s="7" t="s">
+      <c r="G38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H38" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R38" s="7" t="s">
+      <c r="R38" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S38" s="7" t="s">
+      <c r="S38" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T38" s="7" t="s">
+      <c r="T38" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U38" s="7" t="s">
+      <c r="U38" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V38" s="7" t="s">
+      <c r="V38" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="39" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D39" s="8" t="s">
+      <c r="D39" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="6">
-        <v>10</v>
-      </c>
-      <c r="F39" s="6">
+      <c r="E39" s="2">
+        <v>10</v>
+      </c>
+      <c r="F39" s="2">
         <v>98.525000000000006</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G39" s="2">
         <v>98.804000000000002</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H39" s="2">
         <v>98.775999999999996</v>
       </c>
-      <c r="R39" s="8" t="s">
+      <c r="R39" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="S39" s="6">
-        <v>10</v>
-      </c>
-      <c r="T39" s="6">
+      <c r="S39" s="2">
+        <v>10</v>
+      </c>
+      <c r="T39" s="2">
         <v>98.525000000000006</v>
       </c>
-      <c r="U39" s="6">
-        <v>10</v>
-      </c>
-      <c r="V39" s="6">
+      <c r="U39" s="2">
+        <v>10</v>
+      </c>
+      <c r="V39" s="2">
         <v>98.804000000000002</v>
       </c>
     </row>
     <row r="40" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D40" s="8" t="s">
+      <c r="D40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="6">
-        <v>10</v>
-      </c>
-      <c r="F40" s="6">
+      <c r="E40" s="2">
+        <v>10</v>
+      </c>
+      <c r="F40" s="2">
         <v>98.832999999999998</v>
       </c>
-      <c r="G40" s="6">
+      <c r="G40" s="2">
         <v>99.106999999999999</v>
       </c>
-      <c r="H40" s="6">
+      <c r="H40" s="2">
         <v>99.078999999999994</v>
       </c>
-      <c r="R40" s="8" t="s">
+      <c r="R40" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="S40" s="6">
-        <v>10</v>
-      </c>
-      <c r="T40" s="6">
+      <c r="S40" s="2">
+        <v>10</v>
+      </c>
+      <c r="T40" s="2">
         <v>98.832999999999998</v>
       </c>
-      <c r="U40" s="6">
-        <v>10</v>
-      </c>
-      <c r="V40" s="6">
+      <c r="U40" s="2">
+        <v>10</v>
+      </c>
+      <c r="V40" s="2">
         <v>99.106999999999999</v>
       </c>
     </row>
     <row r="41" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D41" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="6">
-        <v>7</v>
-      </c>
-      <c r="F41" s="6">
+      <c r="D41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E41" s="2">
+        <v>7</v>
+      </c>
+      <c r="F41" s="2">
         <v>99.099000000000004</v>
       </c>
-      <c r="G41" s="6">
+      <c r="G41" s="2">
         <v>99.447000000000003</v>
       </c>
-      <c r="H41" s="6">
+      <c r="H41" s="2">
         <v>99.397000000000006</v>
       </c>
-      <c r="R41" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="S41" s="6">
+      <c r="R41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S41" s="2">
         <v>9</v>
       </c>
-      <c r="T41" s="6">
+      <c r="T41" s="2">
         <v>99.108999999999995</v>
       </c>
-      <c r="U41" s="6">
-        <v>7</v>
-      </c>
-      <c r="V41" s="6">
+      <c r="U41" s="2">
+        <v>7</v>
+      </c>
+      <c r="V41" s="2">
         <v>99.447000000000003</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="R37:V37"/>
-    <mergeCell ref="R23:V23"/>
-    <mergeCell ref="R30:V30"/>
-    <mergeCell ref="X23:AB23"/>
-    <mergeCell ref="X30:AB30"/>
+    <mergeCell ref="D37:H37"/>
     <mergeCell ref="R2:V2"/>
     <mergeCell ref="R9:V9"/>
     <mergeCell ref="R16:V16"/>
@@ -1719,7 +1728,11 @@
     <mergeCell ref="D23:H23"/>
     <mergeCell ref="D30:H30"/>
     <mergeCell ref="J23:N23"/>
-    <mergeCell ref="D37:H37"/>
+    <mergeCell ref="R37:V37"/>
+    <mergeCell ref="R23:V23"/>
+    <mergeCell ref="R30:V30"/>
+    <mergeCell ref="X23:AB23"/>
+    <mergeCell ref="X30:AB30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modifyed excel and project book
</commit_message>
<xml_diff>
--- a/Docs/Result Summary.xlsx
+++ b/Docs/Result Summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i560646/Desktop/Eden/ML Final Project/Image_Based_Malware_Classification/Docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ML Cyber\New Repo\Image_Based_Malware_Classification\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04854A8F-06CB-3447-B79E-C7E09B1E5838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AF674B-7846-440D-9E35-ECF50C03C74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -218,6 +218,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -225,9 +228,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -318,7 +318,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IL"/>
+          <a:endParaRPr lang="he-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -447,7 +447,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -465,10 +465,7 @@
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                       <a:round/>
                     </a:ln>
@@ -546,8 +543,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.9383448382625162E-2"/>
-                  <c:y val="3.4931670775195656E-2"/>
+                  <c:x val="-3.9383468008096126E-2"/>
+                  <c:y val="5.1112809927885229E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -590,7 +587,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -608,10 +605,7 @@
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
+                        <a:srgbClr val="7030A0"/>
                       </a:solidFill>
                       <a:round/>
                     </a:ln>
@@ -733,7 +727,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -884,7 +878,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-IL"/>
+              <a:endParaRPr lang="he-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -922,7 +916,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-IL"/>
+            <a:endParaRPr lang="he-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1279963440"/>
@@ -1030,7 +1024,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-IL"/>
+              <a:endParaRPr lang="he-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1062,7 +1056,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-IL"/>
+            <a:endParaRPr lang="he-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1280095088"/>
@@ -1111,7 +1105,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IL"/>
+          <a:endParaRPr lang="he-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1148,7 +1142,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-IL"/>
+      <a:endParaRPr lang="he-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1222,7 +1216,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IL"/>
+          <a:endParaRPr lang="he-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1285,8 +1279,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.4021518087718992E-2"/>
-                  <c:y val="-1.3655075030514831E-2"/>
+                  <c:x val="-7.6929728241657572E-2"/>
+                  <c:y val="9.637718828835716E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1307,8 +1301,8 @@
               <c:idx val="2"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.8811509151168441E-2"/>
-                  <c:y val="-6.5326807553311161E-2"/>
+                  <c:x val="-6.6097935612637326E-2"/>
+                  <c:y val="-4.5909334148765385E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1351,7 +1345,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1369,10 +1363,7 @@
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="accent1"/>
                       </a:solidFill>
                       <a:round/>
                     </a:ln>
@@ -1489,8 +1480,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-3.5808828186021047E-2"/>
-                  <c:y val="-2.8852643419572582E-2"/>
+                  <c:x val="-5.4879105546848418E-2"/>
+                  <c:y val="-3.8561272074000487E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1504,6 +1495,28 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{0000000C-DE4E-E447-B4E6-124D2DC85ABB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-3.4414172602680896E-3"/>
+                  <c:y val="-7.2791325841551374E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000001-0C4F-4794-AB9C-8E4200FA25AB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1533,7 +1546,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1551,10 +1564,7 @@
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="accent2"/>
                       </a:solidFill>
                       <a:round/>
                     </a:ln>
@@ -1674,8 +1684,8 @@
               <c:idx val="1"/>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-1.9723037301302551E-2"/>
-                  <c:y val="4.1056171170093102E-2"/>
+                  <c:x val="7.2932718928607129E-3"/>
+                  <c:y val="3.7819993374614579E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:dLblPos val="r"/>
@@ -1689,6 +1699,28 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                 <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                   <c16:uniqueId val="{00000008-DE4E-E447-B4E6-124D2DC85ABB}"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-1.456577165041509E-2"/>
+                  <c:y val="5.9894758300843461E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:dLblPos val="r"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="1"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+                <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                  <c16:uniqueId val="{00000000-0C4F-4794-AB9C-8E4200FA25AB}"/>
                 </c:ext>
               </c:extLst>
             </c:dLbl>
@@ -1718,7 +1750,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1736,10 +1768,7 @@
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
+                        <a:schemeClr val="accent6"/>
                       </a:solidFill>
                       <a:round/>
                     </a:ln>
@@ -1856,7 +1885,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1985,7 +2014,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-IL"/>
+                <a:endParaRPr lang="he-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2136,7 +2165,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-IL"/>
+              <a:endParaRPr lang="he-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2174,7 +2203,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-IL"/>
+            <a:endParaRPr lang="he-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1279963440"/>
@@ -2274,7 +2303,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-IL"/>
+              <a:endParaRPr lang="he-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2306,7 +2335,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-IL"/>
+            <a:endParaRPr lang="he-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1280095088"/>
@@ -2355,7 +2384,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-IL"/>
+          <a:endParaRPr lang="he-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2392,7 +2421,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-IL"/>
+      <a:endParaRPr lang="he-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3867,53 +3896,53 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF31505B-2C63-644B-873C-2CE4A29A5DA4}">
   <dimension ref="D2:AB41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S41" sqref="S41"/>
+    <sheetView tabSelected="1" topLeftCell="S7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z44" sqref="Z44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.83203125" style="1"/>
+    <col min="1" max="3" width="10.77734375" style="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" style="1"/>
+    <col min="9" max="9" width="10.77734375" style="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1"/>
+    <col min="15" max="15" width="10.77734375" style="1"/>
     <col min="16" max="16" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.83203125" style="1"/>
-    <col min="19" max="19" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="10.77734375" style="1"/>
+    <col min="19" max="19" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.83203125" style="1"/>
+    <col min="29" max="16384" width="10.77734375" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="7"/>
-      <c r="R2" s="8" t="s">
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="8"/>
+      <c r="R2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="8"/>
-      <c r="T2" s="8"/>
-      <c r="U2" s="8"/>
-      <c r="V2" s="8"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
+      <c r="V2" s="5"/>
     </row>
     <row r="3" spans="4:22" x14ac:dyDescent="0.2">
       <c r="D3" s="3" t="s">
@@ -4044,20 +4073,20 @@
       </c>
     </row>
     <row r="9" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7"/>
-      <c r="R9" s="8" t="s">
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
+      <c r="G9" s="7"/>
+      <c r="H9" s="8"/>
+      <c r="R9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="S9" s="8"/>
-      <c r="T9" s="8"/>
-      <c r="U9" s="8"/>
-      <c r="V9" s="8"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
     </row>
     <row r="10" spans="4:22" x14ac:dyDescent="0.2">
       <c r="D10" s="3" t="s">
@@ -4188,20 +4217,20 @@
       </c>
     </row>
     <row r="16" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
-      <c r="R16" s="8" t="s">
+      <c r="E16" s="7"/>
+      <c r="F16" s="7"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="8"/>
+      <c r="R16" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
+      <c r="S16" s="5"/>
+      <c r="T16" s="5"/>
+      <c r="U16" s="5"/>
+      <c r="V16" s="5"/>
     </row>
     <row r="17" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D17" s="3" t="s">
@@ -4332,34 +4361,34 @@
       </c>
     </row>
     <row r="23" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="7"/>
-      <c r="J23" s="5" t="s">
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="8"/>
+      <c r="J23" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
-      <c r="M23" s="6"/>
-      <c r="N23" s="7"/>
-      <c r="R23" s="5" t="s">
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="8"/>
+      <c r="R23" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S23" s="6"/>
-      <c r="T23" s="6"/>
-      <c r="U23" s="6"/>
-      <c r="V23" s="7"/>
-      <c r="X23" s="8" t="s">
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="8"/>
+      <c r="X23" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="8"/>
-      <c r="Z23" s="8"/>
-      <c r="AA23" s="8"/>
-      <c r="AB23" s="8"/>
+      <c r="Y23" s="5"/>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="5"/>
+      <c r="AB23" s="5"/>
     </row>
     <row r="24" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D24" s="3" t="s">
@@ -4610,34 +4639,34 @@
       </c>
     </row>
     <row r="30" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
-      <c r="J30" s="5" t="s">
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="8"/>
+      <c r="J30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
-      <c r="M30" s="6"/>
-      <c r="N30" s="7"/>
-      <c r="R30" s="5" t="s">
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="8"/>
+      <c r="R30" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-      <c r="V30" s="7"/>
-      <c r="X30" s="5" t="s">
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="8"/>
+      <c r="X30" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="Y30" s="6"/>
-      <c r="Z30" s="6"/>
-      <c r="AA30" s="6"/>
-      <c r="AB30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
+      <c r="AB30" s="8"/>
     </row>
     <row r="31" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D31" s="3" t="s">
@@ -4893,20 +4922,20 @@
       </c>
     </row>
     <row r="37" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="7"/>
-      <c r="R37" s="5" t="s">
+      <c r="E37" s="7"/>
+      <c r="F37" s="7"/>
+      <c r="G37" s="7"/>
+      <c r="H37" s="8"/>
+      <c r="R37" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="6"/>
-      <c r="T37" s="6"/>
-      <c r="U37" s="6"/>
-      <c r="V37" s="7"/>
+      <c r="S37" s="7"/>
+      <c r="T37" s="7"/>
+      <c r="U37" s="7"/>
+      <c r="V37" s="8"/>
     </row>
     <row r="38" spans="4:28" x14ac:dyDescent="0.2">
       <c r="D38" s="3" t="s">

</xml_diff>

<commit_message>
[INFRA] update & delete files + update results file
</commit_message>
<xml_diff>
--- a/Docs/Result Summary.xlsx
+++ b/Docs/Result Summary.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\ML Cyber\New Repo\Image_Based_Malware_Classification\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i560646/Desktop/Eden/ML Final Project/Image_Based_Malware_Classification/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9AF674B-7846-440D-9E35-ECF50C03C74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2556FEF4-D69A-0444-BB04-D4AA8FAE3302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="36240" windowHeight="20060" xr2:uid="{0A203DC1-8D7A-5448-A5B0-98BE3735A09B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="25">
   <si>
     <t>LDA</t>
   </si>
@@ -100,6 +100,18 @@
   <si>
     <t>.</t>
   </si>
+  <si>
+    <t>זמני ריצה</t>
+  </si>
+  <si>
+    <t>Time (Minutes)</t>
+  </si>
+  <si>
+    <t>AVG</t>
+  </si>
+  <si>
+    <t>אחוזי הצלחה</t>
+  </si>
 </sst>
 </file>
 
@@ -109,12 +121,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -139,8 +151,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -200,11 +218,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,6 +326,36 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -318,7 +446,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -343,7 +471,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$2</c:f>
+              <c:f>Sheet1!$R$5</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -447,7 +575,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -477,7 +605,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$4:$T$6</c:f>
+              <c:f>Sheet1!$T$7:$T$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -505,7 +633,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$9</c:f>
+              <c:f>Sheet1!$R$12</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -587,7 +715,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -617,7 +745,7 @@
           </c:dLbls>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$11:$T$13</c:f>
+              <c:f>Sheet1!$T$14:$T$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -645,7 +773,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$16</c:f>
+              <c:f>Sheet1!$R$19</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -727,7 +855,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="b"/>
@@ -760,24 +888,24 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$4:$R$6</c:f>
+              <c:f>Sheet1!$R$7:$R$9</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>32x32</c:v>
+                  <c:v>Size</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>64x64</c:v>
+                  <c:v>Size</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>128x128</c:v>
+                  <c:v>Size</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$18:$T$20</c:f>
+              <c:f>Sheet1!$T$21:$T$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -878,7 +1006,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -916,7 +1044,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1279963440"/>
@@ -1024,7 +1152,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1056,7 +1184,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1280095088"/>
@@ -1105,7 +1233,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1142,7 +1270,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1216,7 +1344,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -1241,7 +1369,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$23</c:f>
+              <c:f>Sheet1!$R$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1345,7 +1473,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1375,7 +1503,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$18:$R$20</c:f>
+              <c:f>Sheet1!$R$21:$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1392,7 +1520,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$25:$T$27</c:f>
+              <c:f>Sheet1!$T$28:$T$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1420,7 +1548,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$23</c:f>
+              <c:f>Sheet1!$X$26</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1546,7 +1674,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1576,7 +1704,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$18:$R$20</c:f>
+              <c:f>Sheet1!$R$21:$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1593,7 +1721,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$Z$25:$Z$27</c:f>
+              <c:f>Sheet1!$Z$28:$Z$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1621,7 +1749,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$30</c:f>
+              <c:f>Sheet1!$R$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1750,7 +1878,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1780,7 +1908,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$18:$R$20</c:f>
+              <c:f>Sheet1!$R$21:$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1797,7 +1925,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$32:$T$34</c:f>
+              <c:f>Sheet1!$T$35:$T$37</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -1825,7 +1953,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$X$30</c:f>
+              <c:f>Sheet1!$X$33</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1885,7 +2013,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -1918,7 +2046,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$18:$R$20</c:f>
+              <c:f>Sheet1!$R$21:$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1954,7 +2082,7 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$R$37</c:f>
+              <c:f>Sheet1!$R$40</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2014,7 +2142,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="he-IL"/>
+                <a:endParaRPr lang="en-IL"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="t"/>
@@ -2047,7 +2175,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$R$18:$R$20</c:f>
+              <c:f>Sheet1!$R$21:$R$23</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -2064,7 +2192,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$T$39:$T$41</c:f>
+              <c:f>Sheet1!$T$42:$T$44</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -2165,7 +2293,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2203,7 +2331,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1279963440"/>
@@ -2303,7 +2431,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="he-IL"/>
+              <a:endParaRPr lang="en-IL"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -2335,7 +2463,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="he-IL"/>
+            <a:endParaRPr lang="en-IL"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1280095088"/>
@@ -2384,7 +2512,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="he-IL"/>
+          <a:endParaRPr lang="en-IL"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -2421,7 +2549,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="he-IL"/>
+      <a:endParaRPr lang="en-IL"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -3523,15 +3651,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>715736</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>81642</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>76200</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:colOff>391886</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>195943</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3559,15 +3687,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>28</xdr:col>
-      <xdr:colOff>508000</xdr:colOff>
+      <xdr:colOff>736599</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>192314</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>184150</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:colOff>412749</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>81643</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3894,1195 +4022,3055 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF31505B-2C63-644B-873C-2CE4A29A5DA4}">
-  <dimension ref="D2:AB41"/>
+  <dimension ref="D1:BA82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z44" sqref="Z44"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="AD6" sqref="AD6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.77734375" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="3" width="10.77734375" style="1"/>
+    <col min="1" max="3" width="10.83203125" style="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" style="1"/>
+    <col min="9" max="9" width="10.83203125" style="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="6.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" style="1"/>
+    <col min="15" max="15" width="10.83203125" style="1"/>
     <col min="16" max="16" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="10.77734375" style="1"/>
-    <col min="19" max="19" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="1"/>
+    <col min="18" max="18" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="12.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="12.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="26" max="28" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="10.77734375" style="1"/>
+    <col min="29" max="41" width="10.83203125" style="1"/>
+    <col min="42" max="42" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="43.33203125" style="1" customWidth="1"/>
+    <col min="44" max="45" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="52" width="20.6640625" style="1" customWidth="1"/>
+    <col min="53" max="53" width="8" style="1" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="21.83203125" style="1" customWidth="1"/>
+    <col min="55" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D2" s="6" t="s">
+    <row r="1" spans="4:53" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q2" s="9"/>
+      <c r="R2" s="10"/>
+      <c r="S2" s="10"/>
+      <c r="T2" s="10"/>
+      <c r="U2" s="10"/>
+      <c r="V2" s="10"/>
+      <c r="W2" s="10"/>
+      <c r="X2" s="10"/>
+      <c r="Y2" s="10"/>
+      <c r="Z2" s="10"/>
+      <c r="AA2" s="10"/>
+      <c r="AB2" s="10"/>
+      <c r="AC2" s="10"/>
+      <c r="AD2" s="10"/>
+      <c r="AE2" s="10"/>
+      <c r="AF2" s="10"/>
+      <c r="AG2" s="10"/>
+      <c r="AH2" s="10"/>
+      <c r="AI2" s="10"/>
+      <c r="AJ2" s="10"/>
+      <c r="AK2" s="10"/>
+      <c r="AL2" s="11"/>
+      <c r="AO2" s="9"/>
+      <c r="AP2" s="10"/>
+      <c r="AQ2" s="10"/>
+      <c r="AR2" s="10"/>
+      <c r="AS2" s="10"/>
+      <c r="AT2" s="10"/>
+      <c r="AU2" s="10"/>
+      <c r="AV2" s="10"/>
+      <c r="AW2" s="10"/>
+      <c r="AX2" s="10"/>
+      <c r="AY2" s="10"/>
+      <c r="AZ2" s="10"/>
+      <c r="BA2" s="11"/>
+    </row>
+    <row r="3" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q3" s="12"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
+      <c r="U3" s="13"/>
+      <c r="V3" s="13"/>
+      <c r="W3" s="13"/>
+      <c r="X3" s="13"/>
+      <c r="Y3" s="13"/>
+      <c r="Z3" s="13"/>
+      <c r="AA3" s="13"/>
+      <c r="AB3" s="13"/>
+      <c r="AC3" s="13"/>
+      <c r="AD3" s="13"/>
+      <c r="AE3" s="13"/>
+      <c r="AF3" s="13"/>
+      <c r="AG3" s="13"/>
+      <c r="AH3" s="13"/>
+      <c r="AI3" s="13"/>
+      <c r="AJ3" s="13"/>
+      <c r="AK3" s="13"/>
+      <c r="AL3" s="14"/>
+      <c r="AO3" s="12"/>
+      <c r="AP3" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="AQ3" s="18"/>
+      <c r="AR3" s="18"/>
+      <c r="AS3" s="18"/>
+      <c r="AT3" s="18"/>
+      <c r="AU3" s="18"/>
+      <c r="AV3" s="18"/>
+      <c r="AW3" s="18"/>
+      <c r="AX3" s="18"/>
+      <c r="AY3" s="18"/>
+      <c r="AZ3" s="18"/>
+      <c r="BA3" s="14"/>
+    </row>
+    <row r="4" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D4" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="8"/>
-      <c r="R2" s="5" t="s">
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="8"/>
+      <c r="Q4" s="12"/>
+      <c r="Y4" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="18"/>
+      <c r="AB4" s="18"/>
+      <c r="AC4" s="18"/>
+      <c r="AD4" s="18"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="18"/>
+      <c r="AG4" s="18"/>
+      <c r="AH4" s="18"/>
+      <c r="AI4" s="18"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="14"/>
+      <c r="AO4" s="12"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="13"/>
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="14"/>
+    </row>
+    <row r="5" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-    </row>
-    <row r="3" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D3" s="3" t="s">
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
+      <c r="V5" s="5"/>
+      <c r="W5" s="13"/>
+      <c r="X5" s="13"/>
+      <c r="Y5" s="13"/>
+      <c r="Z5" s="13"/>
+      <c r="AA5" s="13"/>
+      <c r="AB5" s="13"/>
+      <c r="AC5" s="13"/>
+      <c r="AD5" s="13"/>
+      <c r="AE5" s="13"/>
+      <c r="AF5" s="13"/>
+      <c r="AG5" s="13"/>
+      <c r="AH5" s="13"/>
+      <c r="AI5" s="13"/>
+      <c r="AJ5" s="13"/>
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="14"/>
+      <c r="AO5" s="12"/>
+      <c r="AP5" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="8"/>
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="13"/>
+      <c r="AT5" s="13"/>
+      <c r="AU5" s="13"/>
+      <c r="AV5" s="13"/>
+      <c r="AW5" s="13"/>
+      <c r="AX5" s="13"/>
+      <c r="AY5" s="13"/>
+      <c r="AZ5" s="13"/>
+      <c r="BA5" s="14"/>
+    </row>
+    <row r="6" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D6" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6" s="2">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2">
+        <v>96.968999999999994</v>
+      </c>
+      <c r="G6" s="2">
+        <v>98.373000000000005</v>
+      </c>
+      <c r="H6" s="2">
+        <v>98.198999999999998</v>
+      </c>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="S6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V6" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W6" s="13"/>
+      <c r="X6" s="13"/>
+      <c r="Y6" s="13"/>
+      <c r="Z6" s="13"/>
+      <c r="AA6" s="13"/>
+      <c r="AB6" s="13"/>
+      <c r="AC6" s="13"/>
+      <c r="AD6" s="13"/>
+      <c r="AE6" s="13"/>
+      <c r="AF6" s="13"/>
+      <c r="AG6" s="13"/>
+      <c r="AH6" s="13"/>
+      <c r="AI6" s="13"/>
+      <c r="AJ6" s="13"/>
+      <c r="AK6" s="13"/>
+      <c r="AL6" s="14"/>
+      <c r="AO6" s="12"/>
+      <c r="AP6" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR6" s="13"/>
+      <c r="AS6" s="13"/>
+      <c r="AT6" s="13"/>
+      <c r="AU6" s="13"/>
+      <c r="AV6" s="13"/>
+      <c r="AW6" s="13"/>
+      <c r="AX6" s="13"/>
+      <c r="AY6" s="13"/>
+      <c r="AZ6" s="13"/>
+      <c r="BA6" s="14"/>
+    </row>
+    <row r="7" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2">
+        <v>97.346999999999994</v>
+      </c>
+      <c r="G7" s="2">
+        <v>99.933000000000007</v>
+      </c>
+      <c r="H7" s="2">
+        <v>99.674000000000007</v>
+      </c>
+      <c r="Q7" s="12"/>
+      <c r="R7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S7" s="2">
+        <v>6</v>
+      </c>
+      <c r="T7" s="2">
+        <v>97.009</v>
+      </c>
+      <c r="U7" s="2">
+        <v>2</v>
+      </c>
+      <c r="V7" s="2">
+        <v>99.15</v>
+      </c>
+      <c r="W7" s="13"/>
+      <c r="X7" s="13"/>
+      <c r="Y7" s="13"/>
+      <c r="Z7" s="13"/>
+      <c r="AA7" s="13"/>
+      <c r="AB7" s="13"/>
+      <c r="AC7" s="13"/>
+      <c r="AD7" s="13"/>
+      <c r="AE7" s="13"/>
+      <c r="AF7" s="13"/>
+      <c r="AG7" s="13"/>
+      <c r="AH7" s="13"/>
+      <c r="AI7" s="13"/>
+      <c r="AJ7" s="13"/>
+      <c r="AK7" s="13"/>
+      <c r="AL7" s="14"/>
+      <c r="AO7" s="12"/>
+      <c r="AP7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ7" s="2">
+        <v>5.2694999999999999</v>
+      </c>
+      <c r="AR7" s="13"/>
+      <c r="AS7" s="13"/>
+      <c r="AT7" s="13"/>
+      <c r="AU7" s="13"/>
+      <c r="AV7" s="13"/>
+      <c r="AW7" s="13"/>
+      <c r="AX7" s="13"/>
+      <c r="AY7" s="13"/>
+      <c r="AZ7" s="13"/>
+      <c r="BA7" s="14"/>
+    </row>
+    <row r="8" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E8" s="2">
+        <v>10</v>
+      </c>
+      <c r="F8" s="2">
+        <v>65.015000000000001</v>
+      </c>
+      <c r="G8" s="2">
+        <v>100</v>
+      </c>
+      <c r="H8" s="2">
+        <v>96.501000000000005</v>
+      </c>
+      <c r="Q8" s="12"/>
+      <c r="R8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S8" s="2">
+        <v>10</v>
+      </c>
+      <c r="T8" s="2">
+        <v>97.346999999999994</v>
+      </c>
+      <c r="U8" s="2">
+        <v>2</v>
+      </c>
+      <c r="V8" s="2">
+        <v>100</v>
+      </c>
+      <c r="W8" s="13"/>
+      <c r="X8" s="13"/>
+      <c r="Y8" s="13"/>
+      <c r="Z8" s="13"/>
+      <c r="AA8" s="13"/>
+      <c r="AB8" s="13"/>
+      <c r="AC8" s="13"/>
+      <c r="AD8" s="13"/>
+      <c r="AE8" s="13"/>
+      <c r="AF8" s="13"/>
+      <c r="AG8" s="13"/>
+      <c r="AH8" s="13"/>
+      <c r="AI8" s="13"/>
+      <c r="AJ8" s="13"/>
+      <c r="AK8" s="13"/>
+      <c r="AL8" s="14"/>
+      <c r="AO8" s="12"/>
+      <c r="AP8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ8" s="2">
+        <v>82.537800000000004</v>
+      </c>
+      <c r="AR8" s="13"/>
+      <c r="AS8" s="13"/>
+      <c r="AT8" s="13"/>
+      <c r="AU8" s="13"/>
+      <c r="AV8" s="13"/>
+      <c r="AW8" s="13"/>
+      <c r="AX8" s="13"/>
+      <c r="AY8" s="13"/>
+      <c r="AZ8" s="13"/>
+      <c r="BA8" s="14"/>
+    </row>
+    <row r="9" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q9" s="12"/>
+      <c r="R9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S9" s="2">
+        <v>3</v>
+      </c>
+      <c r="T9" s="2">
+        <v>70.73</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V9" s="2">
+        <v>100</v>
+      </c>
+      <c r="W9" s="13"/>
+      <c r="X9" s="13"/>
+      <c r="Y9" s="13"/>
+      <c r="Z9" s="13"/>
+      <c r="AA9" s="13"/>
+      <c r="AB9" s="13"/>
+      <c r="AC9" s="13"/>
+      <c r="AD9" s="13"/>
+      <c r="AE9" s="13"/>
+      <c r="AF9" s="13"/>
+      <c r="AG9" s="13"/>
+      <c r="AH9" s="13"/>
+      <c r="AI9" s="13"/>
+      <c r="AJ9" s="13"/>
+      <c r="AK9" s="13"/>
+      <c r="AL9" s="14"/>
+      <c r="AO9" s="12"/>
+      <c r="AP9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ9" s="2">
+        <v>405.30700000000002</v>
+      </c>
+      <c r="AR9" s="13"/>
+      <c r="AS9" s="13"/>
+      <c r="AT9" s="13"/>
+      <c r="AU9" s="13"/>
+      <c r="AV9" s="13"/>
+      <c r="AW9" s="13"/>
+      <c r="AX9" s="13"/>
+      <c r="AY9" s="13"/>
+      <c r="AZ9" s="13"/>
+      <c r="BA9" s="14"/>
+    </row>
+    <row r="10" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q10" s="12"/>
+      <c r="R10" s="13"/>
+      <c r="S10" s="13"/>
+      <c r="T10" s="13"/>
+      <c r="U10" s="13"/>
+      <c r="V10" s="13"/>
+      <c r="W10" s="13"/>
+      <c r="X10" s="13"/>
+      <c r="Y10" s="13"/>
+      <c r="Z10" s="13"/>
+      <c r="AA10" s="13"/>
+      <c r="AB10" s="13"/>
+      <c r="AC10" s="13"/>
+      <c r="AD10" s="13"/>
+      <c r="AE10" s="13"/>
+      <c r="AF10" s="13"/>
+      <c r="AG10" s="13"/>
+      <c r="AH10" s="13"/>
+      <c r="AI10" s="13"/>
+      <c r="AJ10" s="13"/>
+      <c r="AK10" s="13"/>
+      <c r="AL10" s="14"/>
+      <c r="AO10" s="12"/>
+      <c r="AP10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ10" s="2">
+        <f>AVERAGE(AQ7:AQ9)</f>
+        <v>164.37143333333333</v>
+      </c>
+      <c r="AR10" s="13"/>
+      <c r="AS10" s="13"/>
+      <c r="AT10" s="13"/>
+      <c r="AU10" s="13"/>
+      <c r="AV10" s="13"/>
+      <c r="AW10" s="13"/>
+      <c r="AX10" s="13"/>
+      <c r="AY10" s="13"/>
+      <c r="AZ10" s="13"/>
+      <c r="BA10" s="14"/>
+    </row>
+    <row r="11" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="7"/>
+      <c r="F11" s="7"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="8"/>
+      <c r="Q11" s="12"/>
+      <c r="R11" s="13"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="13"/>
+      <c r="X11" s="13"/>
+      <c r="Y11" s="13"/>
+      <c r="Z11" s="13"/>
+      <c r="AA11" s="13"/>
+      <c r="AB11" s="13"/>
+      <c r="AC11" s="13"/>
+      <c r="AD11" s="13"/>
+      <c r="AE11" s="13"/>
+      <c r="AF11" s="13"/>
+      <c r="AG11" s="13"/>
+      <c r="AH11" s="13"/>
+      <c r="AI11" s="13"/>
+      <c r="AJ11" s="13"/>
+      <c r="AK11" s="13"/>
+      <c r="AL11" s="14"/>
+      <c r="AO11" s="12"/>
+      <c r="AP11" s="13"/>
+      <c r="AQ11" s="13"/>
+      <c r="AR11" s="13"/>
+      <c r="AS11" s="13"/>
+      <c r="AT11" s="13"/>
+      <c r="AU11" s="13"/>
+      <c r="AV11" s="13"/>
+      <c r="AW11" s="13"/>
+      <c r="AX11" s="13"/>
+      <c r="AY11" s="13"/>
+      <c r="AZ11" s="13"/>
+      <c r="BA11" s="14"/>
+    </row>
+    <row r="12" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="3" t="s">
+      <c r="Q12" s="12"/>
+      <c r="R12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="13"/>
+      <c r="X12" s="13"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="13"/>
+      <c r="AC12" s="13"/>
+      <c r="AD12" s="13"/>
+      <c r="AE12" s="13"/>
+      <c r="AF12" s="13"/>
+      <c r="AG12" s="13"/>
+      <c r="AH12" s="13"/>
+      <c r="AI12" s="13"/>
+      <c r="AJ12" s="13"/>
+      <c r="AK12" s="13"/>
+      <c r="AL12" s="14"/>
+      <c r="AO12" s="12"/>
+      <c r="AP12" s="13"/>
+      <c r="AQ12" s="13"/>
+      <c r="AR12" s="13"/>
+      <c r="AS12" s="13"/>
+      <c r="AT12" s="13"/>
+      <c r="AU12" s="13"/>
+      <c r="AV12" s="13"/>
+      <c r="AW12" s="13"/>
+      <c r="AX12" s="13"/>
+      <c r="AY12" s="13"/>
+      <c r="AZ12" s="13"/>
+      <c r="BA12" s="14"/>
+    </row>
+    <row r="13" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D13" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13" s="2">
+        <v>6</v>
+      </c>
+      <c r="F13" s="2">
+        <v>95.238</v>
+      </c>
+      <c r="G13" s="2">
+        <v>95.459000000000003</v>
+      </c>
+      <c r="H13" s="2">
+        <v>95.421999999999997</v>
+      </c>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="3" t="s">
+      <c r="S13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="T3" s="3" t="s">
+      <c r="T13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="U3" s="3" t="s">
+      <c r="U13" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="V13" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D4" s="4" t="s">
+      <c r="W13" s="13"/>
+      <c r="X13" s="13"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="13"/>
+      <c r="AC13" s="13"/>
+      <c r="AD13" s="13"/>
+      <c r="AE13" s="13"/>
+      <c r="AF13" s="13"/>
+      <c r="AG13" s="13"/>
+      <c r="AH13" s="13"/>
+      <c r="AI13" s="13"/>
+      <c r="AJ13" s="13"/>
+      <c r="AK13" s="13"/>
+      <c r="AL13" s="14"/>
+      <c r="AO13" s="12"/>
+      <c r="AP13" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="AQ13" s="8"/>
+      <c r="AR13" s="13"/>
+      <c r="AS13" s="13"/>
+      <c r="AT13" s="13"/>
+      <c r="AU13" s="13"/>
+      <c r="AV13" s="13"/>
+      <c r="AW13" s="13"/>
+      <c r="AX13" s="13"/>
+      <c r="AY13" s="13"/>
+      <c r="AZ13" s="13"/>
+      <c r="BA13" s="14"/>
+    </row>
+    <row r="14" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="2">
+        <v>3</v>
+      </c>
+      <c r="F14" s="2">
+        <v>96.466999999999999</v>
+      </c>
+      <c r="G14" s="2">
+        <v>96.881</v>
+      </c>
+      <c r="H14" s="2">
+        <v>96.742999999999995</v>
+      </c>
+      <c r="Q14" s="12"/>
+      <c r="R14" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="2">
+      <c r="S14" s="2">
+        <v>9</v>
+      </c>
+      <c r="T14" s="2">
+        <v>95.257999999999996</v>
+      </c>
+      <c r="U14" s="2">
+        <v>2</v>
+      </c>
+      <c r="V14" s="2">
+        <v>95.677999999999997</v>
+      </c>
+      <c r="W14" s="13"/>
+      <c r="X14" s="13"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="13"/>
+      <c r="AC14" s="13"/>
+      <c r="AD14" s="13"/>
+      <c r="AE14" s="13"/>
+      <c r="AF14" s="13"/>
+      <c r="AG14" s="13"/>
+      <c r="AH14" s="13"/>
+      <c r="AI14" s="13"/>
+      <c r="AJ14" s="13"/>
+      <c r="AK14" s="13"/>
+      <c r="AL14" s="14"/>
+      <c r="AO14" s="12"/>
+      <c r="AP14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ14" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR14" s="13"/>
+      <c r="AS14" s="13"/>
+      <c r="AT14" s="13"/>
+      <c r="AU14" s="13"/>
+      <c r="AV14" s="13"/>
+      <c r="AW14" s="13"/>
+      <c r="AX14" s="13"/>
+      <c r="AY14" s="13"/>
+      <c r="AZ14" s="13"/>
+      <c r="BA14" s="14"/>
+    </row>
+    <row r="15" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E15" s="2">
+        <v>9</v>
+      </c>
+      <c r="F15" s="2">
+        <v>96.885999999999996</v>
+      </c>
+      <c r="G15" s="2">
+        <v>97.299000000000007</v>
+      </c>
+      <c r="H15" s="2">
+        <v>97.253</v>
+      </c>
+      <c r="Q15" s="12"/>
+      <c r="R15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S15" s="2">
+        <v>3</v>
+      </c>
+      <c r="T15" s="2">
+        <v>96.466999999999999</v>
+      </c>
+      <c r="U15" s="2">
+        <v>2</v>
+      </c>
+      <c r="V15" s="2">
+        <v>97.111000000000004</v>
+      </c>
+      <c r="W15" s="13"/>
+      <c r="X15" s="13"/>
+      <c r="Y15" s="13"/>
+      <c r="Z15" s="13"/>
+      <c r="AA15" s="13"/>
+      <c r="AB15" s="13"/>
+      <c r="AC15" s="13"/>
+      <c r="AD15" s="13"/>
+      <c r="AE15" s="13"/>
+      <c r="AF15" s="13"/>
+      <c r="AG15" s="13"/>
+      <c r="AH15" s="13"/>
+      <c r="AI15" s="13"/>
+      <c r="AJ15" s="13"/>
+      <c r="AK15" s="13"/>
+      <c r="AL15" s="14"/>
+      <c r="AO15" s="12"/>
+      <c r="AP15" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ15" s="2">
+        <v>2.4952999999999999</v>
+      </c>
+      <c r="AR15" s="13"/>
+      <c r="AS15" s="13"/>
+      <c r="AT15" s="13"/>
+      <c r="AU15" s="13"/>
+      <c r="AV15" s="13"/>
+      <c r="AW15" s="13"/>
+      <c r="AX15" s="13"/>
+      <c r="AY15" s="13"/>
+      <c r="AZ15" s="13"/>
+      <c r="BA15" s="14"/>
+    </row>
+    <row r="16" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q16" s="12"/>
+      <c r="R16" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S16" s="2">
+        <v>3</v>
+      </c>
+      <c r="T16" s="2">
+        <v>96.887</v>
+      </c>
+      <c r="U16" s="2">
+        <v>2</v>
+      </c>
+      <c r="V16" s="2">
+        <v>97.634</v>
+      </c>
+      <c r="W16" s="13"/>
+      <c r="X16" s="13"/>
+      <c r="Y16" s="13"/>
+      <c r="Z16" s="13"/>
+      <c r="AA16" s="13"/>
+      <c r="AB16" s="13"/>
+      <c r="AC16" s="13"/>
+      <c r="AD16" s="13"/>
+      <c r="AE16" s="13"/>
+      <c r="AF16" s="13"/>
+      <c r="AG16" s="13"/>
+      <c r="AH16" s="13"/>
+      <c r="AI16" s="13"/>
+      <c r="AJ16" s="13"/>
+      <c r="AK16" s="13"/>
+      <c r="AL16" s="14"/>
+      <c r="AO16" s="12"/>
+      <c r="AP16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ16" s="2">
+        <v>6.4211999999999998</v>
+      </c>
+      <c r="AR16" s="13"/>
+      <c r="AS16" s="13"/>
+      <c r="AT16" s="13"/>
+      <c r="AU16" s="13"/>
+      <c r="AV16" s="13"/>
+      <c r="AW16" s="13"/>
+      <c r="AX16" s="13"/>
+      <c r="AY16" s="13"/>
+      <c r="AZ16" s="13"/>
+      <c r="BA16" s="14"/>
+    </row>
+    <row r="17" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q17" s="12"/>
+      <c r="R17" s="13"/>
+      <c r="S17" s="13"/>
+      <c r="T17" s="13"/>
+      <c r="U17" s="13"/>
+      <c r="V17" s="13"/>
+      <c r="W17" s="13"/>
+      <c r="X17" s="13"/>
+      <c r="Y17" s="13"/>
+      <c r="Z17" s="13"/>
+      <c r="AA17" s="13"/>
+      <c r="AB17" s="13"/>
+      <c r="AC17" s="13"/>
+      <c r="AD17" s="13"/>
+      <c r="AE17" s="13"/>
+      <c r="AF17" s="13"/>
+      <c r="AG17" s="13"/>
+      <c r="AH17" s="13"/>
+      <c r="AI17" s="13"/>
+      <c r="AJ17" s="13"/>
+      <c r="AK17" s="13"/>
+      <c r="AL17" s="14"/>
+      <c r="AO17" s="12"/>
+      <c r="AP17" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ17" s="2">
+        <v>28.209599999999998</v>
+      </c>
+      <c r="AR17" s="13"/>
+      <c r="AS17" s="13"/>
+      <c r="AT17" s="13"/>
+      <c r="AU17" s="13"/>
+      <c r="AV17" s="13"/>
+      <c r="AW17" s="13"/>
+      <c r="AX17" s="13"/>
+      <c r="AY17" s="13"/>
+      <c r="AZ17" s="13"/>
+      <c r="BA17" s="14"/>
+    </row>
+    <row r="18" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="7"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="8"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="13"/>
+      <c r="S18" s="13"/>
+      <c r="T18" s="13"/>
+      <c r="U18" s="13"/>
+      <c r="V18" s="13"/>
+      <c r="W18" s="13"/>
+      <c r="X18" s="13"/>
+      <c r="Y18" s="13"/>
+      <c r="Z18" s="13"/>
+      <c r="AA18" s="13"/>
+      <c r="AB18" s="13"/>
+      <c r="AC18" s="13"/>
+      <c r="AD18" s="13"/>
+      <c r="AE18" s="13"/>
+      <c r="AF18" s="13"/>
+      <c r="AG18" s="13"/>
+      <c r="AH18" s="13"/>
+      <c r="AI18" s="13"/>
+      <c r="AJ18" s="13"/>
+      <c r="AK18" s="13"/>
+      <c r="AL18" s="14"/>
+      <c r="AO18" s="12"/>
+      <c r="AP18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ18" s="2">
+        <f>AVERAGE(AQ15:AQ17)</f>
+        <v>12.375366666666665</v>
+      </c>
+      <c r="AR18" s="13"/>
+      <c r="AS18" s="13"/>
+      <c r="AT18" s="13"/>
+      <c r="AU18" s="13"/>
+      <c r="AV18" s="13"/>
+      <c r="AW18" s="13"/>
+      <c r="AX18" s="13"/>
+      <c r="AY18" s="13"/>
+      <c r="AZ18" s="13"/>
+      <c r="BA18" s="14"/>
+    </row>
+    <row r="19" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="2">
-        <v>96.968999999999994</v>
-      </c>
-      <c r="G4" s="2">
-        <v>98.373000000000005</v>
-      </c>
-      <c r="H4" s="2">
-        <v>98.198999999999998</v>
-      </c>
-      <c r="R4" s="4" t="s">
+      <c r="Q19" s="12"/>
+      <c r="R19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="8"/>
+      <c r="W19" s="13"/>
+      <c r="X19" s="13"/>
+      <c r="Y19" s="13"/>
+      <c r="Z19" s="13"/>
+      <c r="AA19" s="13"/>
+      <c r="AB19" s="13"/>
+      <c r="AC19" s="13"/>
+      <c r="AD19" s="13"/>
+      <c r="AE19" s="13"/>
+      <c r="AF19" s="13"/>
+      <c r="AG19" s="13"/>
+      <c r="AH19" s="13"/>
+      <c r="AI19" s="13"/>
+      <c r="AJ19" s="13"/>
+      <c r="AK19" s="13"/>
+      <c r="AL19" s="14"/>
+      <c r="AO19" s="12"/>
+      <c r="AP19" s="13"/>
+      <c r="AQ19" s="13"/>
+      <c r="AR19" s="13"/>
+      <c r="AS19" s="13"/>
+      <c r="AT19" s="13"/>
+      <c r="AU19" s="13"/>
+      <c r="AV19" s="13"/>
+      <c r="AW19" s="13"/>
+      <c r="AX19" s="13"/>
+      <c r="AY19" s="13"/>
+      <c r="AZ19" s="13"/>
+      <c r="BA19" s="14"/>
+    </row>
+    <row r="20" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D20" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="S4" s="2">
-        <v>6</v>
-      </c>
-      <c r="T4" s="2">
-        <v>97.009</v>
-      </c>
-      <c r="U4" s="2">
-        <v>2</v>
-      </c>
-      <c r="V4" s="2">
-        <v>99.15</v>
-      </c>
-    </row>
-    <row r="5" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E5" s="2">
-        <v>10</v>
-      </c>
-      <c r="F5" s="2">
-        <v>97.346999999999994</v>
-      </c>
-      <c r="G5" s="2">
-        <v>99.933000000000007</v>
-      </c>
-      <c r="H5" s="2">
-        <v>99.674000000000007</v>
-      </c>
-      <c r="R5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S5" s="2">
-        <v>10</v>
-      </c>
-      <c r="T5" s="2">
-        <v>97.346999999999994</v>
-      </c>
-      <c r="U5" s="2">
-        <v>2</v>
-      </c>
-      <c r="V5" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="2">
-        <v>10</v>
-      </c>
-      <c r="F6" s="2">
-        <v>65.015000000000001</v>
-      </c>
-      <c r="G6" s="2">
-        <v>100</v>
-      </c>
-      <c r="H6" s="2">
-        <v>96.501000000000005</v>
-      </c>
-      <c r="R6" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S6" s="2">
-        <v>3</v>
-      </c>
-      <c r="T6" s="2">
-        <v>70.73</v>
-      </c>
-      <c r="U6" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V6" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="8"/>
-      <c r="R9" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="S9" s="5"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="5"/>
-      <c r="V9" s="5"/>
-    </row>
-    <row r="10" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V10" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11" s="2">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2">
-        <v>95.238</v>
-      </c>
-      <c r="G11" s="2">
-        <v>95.459000000000003</v>
-      </c>
-      <c r="H11" s="2">
-        <v>95.421999999999997</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S11" s="2">
-        <v>9</v>
-      </c>
-      <c r="T11" s="2">
-        <v>95.257999999999996</v>
-      </c>
-      <c r="U11" s="2">
-        <v>2</v>
-      </c>
-      <c r="V11" s="2">
-        <v>95.677999999999997</v>
-      </c>
-    </row>
-    <row r="12" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E12" s="2">
-        <v>3</v>
-      </c>
-      <c r="F12" s="2">
-        <v>96.466999999999999</v>
-      </c>
-      <c r="G12" s="2">
-        <v>96.881</v>
-      </c>
-      <c r="H12" s="2">
-        <v>96.742999999999995</v>
-      </c>
-      <c r="R12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S12" s="2">
-        <v>3</v>
-      </c>
-      <c r="T12" s="2">
-        <v>96.466999999999999</v>
-      </c>
-      <c r="U12" s="2">
-        <v>2</v>
-      </c>
-      <c r="V12" s="2">
-        <v>97.111000000000004</v>
-      </c>
-    </row>
-    <row r="13" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E13" s="2">
-        <v>9</v>
-      </c>
-      <c r="F13" s="2">
-        <v>96.885999999999996</v>
-      </c>
-      <c r="G13" s="2">
-        <v>97.299000000000007</v>
-      </c>
-      <c r="H13" s="2">
-        <v>97.253</v>
-      </c>
-      <c r="R13" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S13" s="2">
-        <v>3</v>
-      </c>
-      <c r="T13" s="2">
-        <v>96.887</v>
-      </c>
-      <c r="U13" s="2">
-        <v>2</v>
-      </c>
-      <c r="V13" s="2">
-        <v>97.634</v>
-      </c>
-    </row>
-    <row r="16" spans="4:22" x14ac:dyDescent="0.2">
-      <c r="D16" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="8"/>
-      <c r="R16" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="S16" s="5"/>
-      <c r="T16" s="5"/>
-      <c r="U16" s="5"/>
-      <c r="V16" s="5"/>
-    </row>
-    <row r="17" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R17" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S17" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U17" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V17" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <v>10</v>
-      </c>
-      <c r="F18" s="1">
-        <v>58.223999999999997</v>
-      </c>
-      <c r="G18" s="2">
-        <v>93.820999999999998</v>
-      </c>
-      <c r="H18" s="2">
-        <v>90.260999999999996</v>
-      </c>
-      <c r="R18" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="2">
-        <v>10</v>
-      </c>
-      <c r="T18" s="2">
-        <v>58.223999999999997</v>
-      </c>
-      <c r="U18" s="2">
-        <v>2</v>
-      </c>
-      <c r="V18" s="2">
-        <v>96.814999999999998</v>
-      </c>
-    </row>
-    <row r="19" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E19" s="2">
-        <v>10</v>
-      </c>
-      <c r="F19" s="2">
-        <v>50.307000000000002</v>
-      </c>
-      <c r="G19" s="2">
-        <v>100</v>
-      </c>
-      <c r="H19" s="2">
-        <v>95.031000000000006</v>
-      </c>
-      <c r="R19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S19" s="2">
-        <v>4</v>
-      </c>
-      <c r="T19" s="2">
-        <v>54.914999999999999</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="V19" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D20" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="E20" s="2">
         <v>10</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
+        <v>58.223999999999997</v>
+      </c>
+      <c r="G20" s="2">
+        <v>93.820999999999998</v>
+      </c>
+      <c r="H20" s="2">
+        <v>90.260999999999996</v>
+      </c>
+      <c r="Q20" s="12"/>
+      <c r="R20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T20" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W20" s="13"/>
+      <c r="X20" s="13"/>
+      <c r="Y20" s="13"/>
+      <c r="Z20" s="13"/>
+      <c r="AA20" s="13"/>
+      <c r="AB20" s="13"/>
+      <c r="AC20" s="13"/>
+      <c r="AD20" s="13"/>
+      <c r="AE20" s="13"/>
+      <c r="AF20" s="13"/>
+      <c r="AG20" s="13"/>
+      <c r="AH20" s="13"/>
+      <c r="AI20" s="13"/>
+      <c r="AJ20" s="13"/>
+      <c r="AK20" s="13"/>
+      <c r="AL20" s="14"/>
+      <c r="AO20" s="12"/>
+      <c r="AP20" s="13"/>
+      <c r="AQ20" s="13"/>
+      <c r="AR20" s="13"/>
+      <c r="AS20" s="13"/>
+      <c r="AT20" s="13"/>
+      <c r="AU20" s="13"/>
+      <c r="AV20" s="13"/>
+      <c r="AW20" s="13"/>
+      <c r="AX20" s="13"/>
+      <c r="AY20" s="13"/>
+      <c r="AZ20" s="13"/>
+      <c r="BA20" s="14"/>
+    </row>
+    <row r="21" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D21" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E21" s="2">
+        <v>10</v>
+      </c>
+      <c r="F21" s="2">
+        <v>50.307000000000002</v>
+      </c>
+      <c r="G21" s="2">
+        <v>100</v>
+      </c>
+      <c r="H21" s="2">
+        <v>95.031000000000006</v>
+      </c>
+      <c r="Q21" s="12"/>
+      <c r="R21" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="2">
+        <v>10</v>
+      </c>
+      <c r="T21" s="2">
+        <v>58.223999999999997</v>
+      </c>
+      <c r="U21" s="2">
+        <v>2</v>
+      </c>
+      <c r="V21" s="2">
+        <v>96.814999999999998</v>
+      </c>
+      <c r="W21" s="13"/>
+      <c r="X21" s="13"/>
+      <c r="Y21" s="13"/>
+      <c r="Z21" s="13"/>
+      <c r="AA21" s="13"/>
+      <c r="AB21" s="13"/>
+      <c r="AC21" s="13"/>
+      <c r="AD21" s="13"/>
+      <c r="AE21" s="13"/>
+      <c r="AF21" s="13"/>
+      <c r="AG21" s="13"/>
+      <c r="AH21" s="13"/>
+      <c r="AI21" s="13"/>
+      <c r="AJ21" s="13"/>
+      <c r="AK21" s="13"/>
+      <c r="AL21" s="14"/>
+      <c r="AO21" s="12"/>
+      <c r="AP21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="AQ21" s="8"/>
+      <c r="AR21" s="13"/>
+      <c r="AS21" s="13"/>
+      <c r="AT21" s="13"/>
+      <c r="AU21" s="13"/>
+      <c r="AV21" s="13"/>
+      <c r="AW21" s="13"/>
+      <c r="AX21" s="13"/>
+      <c r="AY21" s="13"/>
+      <c r="AZ21" s="13"/>
+      <c r="BA21" s="14"/>
+    </row>
+    <row r="22" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D22" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E22" s="2">
+        <v>10</v>
+      </c>
+      <c r="F22" s="2">
         <v>48.884</v>
       </c>
-      <c r="G20" s="2">
+      <c r="G22" s="2">
         <v>100</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H22" s="2">
         <v>94.888000000000005</v>
       </c>
-      <c r="R20" s="4" t="s">
+      <c r="Q22" s="12"/>
+      <c r="R22" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S22" s="2">
+        <v>4</v>
+      </c>
+      <c r="T22" s="2">
+        <v>54.914999999999999</v>
+      </c>
+      <c r="U22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="V22" s="2">
+        <v>100</v>
+      </c>
+      <c r="W22" s="13"/>
+      <c r="X22" s="13"/>
+      <c r="Y22" s="13"/>
+      <c r="Z22" s="13"/>
+      <c r="AA22" s="13"/>
+      <c r="AB22" s="13"/>
+      <c r="AC22" s="13"/>
+      <c r="AD22" s="13"/>
+      <c r="AE22" s="13"/>
+      <c r="AF22" s="13"/>
+      <c r="AG22" s="13"/>
+      <c r="AH22" s="13"/>
+      <c r="AI22" s="13"/>
+      <c r="AJ22" s="13"/>
+      <c r="AK22" s="13"/>
+      <c r="AL22" s="14"/>
+      <c r="AO22" s="12"/>
+      <c r="AP22" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR22" s="13"/>
+      <c r="AS22" s="13"/>
+      <c r="AT22" s="13"/>
+      <c r="AU22" s="13"/>
+      <c r="AV22" s="13"/>
+      <c r="AW22" s="13"/>
+      <c r="AX22" s="13"/>
+      <c r="AY22" s="13"/>
+      <c r="AZ22" s="13"/>
+      <c r="BA22" s="14"/>
+    </row>
+    <row r="23" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q23" s="12"/>
+      <c r="R23" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S20" s="2">
+      <c r="S23" s="2">
         <v>7</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T23" s="2">
         <v>48.975999999999999</v>
       </c>
-      <c r="U20" s="2" t="s">
+      <c r="U23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V20" s="2">
+      <c r="V23" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="23" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D23" s="6" t="s">
+      <c r="W23" s="13"/>
+      <c r="X23" s="13"/>
+      <c r="Y23" s="13"/>
+      <c r="Z23" s="13"/>
+      <c r="AA23" s="13"/>
+      <c r="AB23" s="13"/>
+      <c r="AC23" s="13"/>
+      <c r="AD23" s="13"/>
+      <c r="AE23" s="13"/>
+      <c r="AF23" s="13"/>
+      <c r="AG23" s="13"/>
+      <c r="AH23" s="13"/>
+      <c r="AI23" s="13"/>
+      <c r="AJ23" s="13"/>
+      <c r="AK23" s="13"/>
+      <c r="AL23" s="14"/>
+      <c r="AO23" s="12"/>
+      <c r="AP23" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ23" s="2">
+        <v>7.3962000000000003</v>
+      </c>
+      <c r="AR23" s="13"/>
+      <c r="AS23" s="13"/>
+      <c r="AT23" s="13"/>
+      <c r="AU23" s="13"/>
+      <c r="AV23" s="13"/>
+      <c r="AW23" s="13"/>
+      <c r="AX23" s="13"/>
+      <c r="AY23" s="13"/>
+      <c r="AZ23" s="13"/>
+      <c r="BA23" s="14"/>
+    </row>
+    <row r="24" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q24" s="12"/>
+      <c r="R24" s="13"/>
+      <c r="S24" s="13"/>
+      <c r="T24" s="13"/>
+      <c r="U24" s="13"/>
+      <c r="V24" s="13"/>
+      <c r="W24" s="13"/>
+      <c r="X24" s="13"/>
+      <c r="Y24" s="13"/>
+      <c r="Z24" s="13"/>
+      <c r="AA24" s="13"/>
+      <c r="AB24" s="13"/>
+      <c r="AC24" s="13"/>
+      <c r="AD24" s="13"/>
+      <c r="AE24" s="13"/>
+      <c r="AF24" s="13"/>
+      <c r="AG24" s="13"/>
+      <c r="AH24" s="13"/>
+      <c r="AI24" s="13"/>
+      <c r="AJ24" s="13"/>
+      <c r="AK24" s="13"/>
+      <c r="AL24" s="14"/>
+      <c r="AO24" s="12"/>
+      <c r="AP24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ24" s="2">
+        <v>51.4114</v>
+      </c>
+      <c r="AR24" s="13"/>
+      <c r="AS24" s="13"/>
+      <c r="AT24" s="13"/>
+      <c r="AU24" s="13"/>
+      <c r="AV24" s="13"/>
+      <c r="AW24" s="13"/>
+      <c r="AX24" s="13"/>
+      <c r="AY24" s="13"/>
+      <c r="AZ24" s="13"/>
+      <c r="BA24" s="14"/>
+    </row>
+    <row r="25" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D25" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="8"/>
-      <c r="J23" s="6" t="s">
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="8"/>
+      <c r="J25" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K23" s="7"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="7"/>
-      <c r="N23" s="8"/>
-      <c r="R23" s="6" t="s">
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="8"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="13"/>
+      <c r="S25" s="13"/>
+      <c r="T25" s="13"/>
+      <c r="U25" s="13"/>
+      <c r="V25" s="13"/>
+      <c r="W25" s="13"/>
+      <c r="X25" s="13"/>
+      <c r="Y25" s="13"/>
+      <c r="Z25" s="13"/>
+      <c r="AA25" s="13"/>
+      <c r="AB25" s="13"/>
+      <c r="AC25" s="13"/>
+      <c r="AD25" s="13"/>
+      <c r="AE25" s="13"/>
+      <c r="AF25" s="13"/>
+      <c r="AG25" s="13"/>
+      <c r="AH25" s="13"/>
+      <c r="AI25" s="13"/>
+      <c r="AJ25" s="13"/>
+      <c r="AK25" s="13"/>
+      <c r="AL25" s="14"/>
+      <c r="AO25" s="12"/>
+      <c r="AP25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ25" s="2">
+        <v>256.59190000000001</v>
+      </c>
+      <c r="AR25" s="13"/>
+      <c r="AS25" s="13"/>
+      <c r="AT25" s="13"/>
+      <c r="AU25" s="13"/>
+      <c r="AV25" s="13"/>
+      <c r="AW25" s="13"/>
+      <c r="AX25" s="13"/>
+      <c r="AY25" s="13"/>
+      <c r="AZ25" s="13"/>
+      <c r="BA25" s="14"/>
+    </row>
+    <row r="26" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="N26" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="S23" s="7"/>
-      <c r="T23" s="7"/>
-      <c r="U23" s="7"/>
-      <c r="V23" s="8"/>
-      <c r="X23" s="5" t="s">
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="8"/>
+      <c r="W26" s="13"/>
+      <c r="X26" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="Y23" s="5"/>
-      <c r="Z23" s="5"/>
-      <c r="AA23" s="5"/>
-      <c r="AB23" s="5"/>
-    </row>
-    <row r="24" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D24" s="3" t="s">
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
+      <c r="AB26" s="8"/>
+      <c r="AC26" s="13"/>
+      <c r="AD26" s="13"/>
+      <c r="AE26" s="13"/>
+      <c r="AF26" s="13"/>
+      <c r="AG26" s="13"/>
+      <c r="AH26" s="13"/>
+      <c r="AI26" s="13"/>
+      <c r="AJ26" s="13"/>
+      <c r="AK26" s="13"/>
+      <c r="AL26" s="14"/>
+      <c r="AO26" s="12"/>
+      <c r="AP26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ26" s="2">
+        <f>AVERAGE(AQ23:AQ25)</f>
+        <v>105.13316666666667</v>
+      </c>
+      <c r="AR26" s="13"/>
+      <c r="AS26" s="13"/>
+      <c r="AT26" s="13"/>
+      <c r="AU26" s="13"/>
+      <c r="AV26" s="13"/>
+      <c r="AW26" s="13"/>
+      <c r="AX26" s="13"/>
+      <c r="AY26" s="13"/>
+      <c r="AZ26" s="13"/>
+      <c r="BA26" s="14"/>
+    </row>
+    <row r="27" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27" s="2">
+        <v>8</v>
+      </c>
+      <c r="F27" s="2">
+        <v>98.71</v>
+      </c>
+      <c r="G27" s="2">
+        <v>99.188000000000002</v>
+      </c>
+      <c r="H27" s="2">
+        <v>99.128</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K27" s="2">
+        <v>10</v>
+      </c>
+      <c r="L27" s="2">
+        <v>99.15</v>
+      </c>
+      <c r="M27" s="2">
+        <v>99.465999999999994</v>
+      </c>
+      <c r="N27" s="2">
+        <v>99.435000000000002</v>
+      </c>
+      <c r="Q27" s="12"/>
+      <c r="R27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="S27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W27" s="13"/>
+      <c r="X27" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z27" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB27" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC27" s="13"/>
+      <c r="AD27" s="13"/>
+      <c r="AE27" s="13"/>
+      <c r="AF27" s="13"/>
+      <c r="AG27" s="13"/>
+      <c r="AH27" s="13"/>
+      <c r="AI27" s="13"/>
+      <c r="AJ27" s="13"/>
+      <c r="AK27" s="13"/>
+      <c r="AL27" s="14"/>
+      <c r="AO27" s="12"/>
+      <c r="AP27" s="13"/>
+      <c r="AQ27" s="13"/>
+      <c r="AR27" s="13"/>
+      <c r="AS27" s="13"/>
+      <c r="AT27" s="13"/>
+      <c r="AU27" s="13"/>
+      <c r="AV27" s="13"/>
+      <c r="AW27" s="13"/>
+      <c r="AX27" s="13"/>
+      <c r="AY27" s="13"/>
+      <c r="AZ27" s="13"/>
+      <c r="BA27" s="14"/>
+    </row>
+    <row r="28" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="2">
+        <v>8</v>
+      </c>
+      <c r="F28" s="2">
+        <v>99.754000000000005</v>
+      </c>
+      <c r="G28" s="2">
+        <v>99.997</v>
+      </c>
+      <c r="H28" s="2">
+        <v>99.966999999999999</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="2">
+        <v>10</v>
+      </c>
+      <c r="L28" s="2">
+        <v>99.825999999999993</v>
+      </c>
+      <c r="M28" s="2">
+        <v>100</v>
+      </c>
+      <c r="N28" s="2">
+        <v>99.983000000000004</v>
+      </c>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S28" s="2">
+        <v>8</v>
+      </c>
+      <c r="T28" s="2">
+        <v>98.71</v>
+      </c>
+      <c r="U28" s="2">
+        <v>8</v>
+      </c>
+      <c r="V28" s="2">
+        <v>99.188000000000002</v>
+      </c>
+      <c r="W28" s="13"/>
+      <c r="X28" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y28" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z28" s="2">
+        <v>99.15</v>
+      </c>
+      <c r="AA28" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB28" s="2">
+        <v>99.465999999999994</v>
+      </c>
+      <c r="AC28" s="13"/>
+      <c r="AD28" s="13"/>
+      <c r="AE28" s="13"/>
+      <c r="AF28" s="13"/>
+      <c r="AG28" s="13"/>
+      <c r="AH28" s="13"/>
+      <c r="AI28" s="13"/>
+      <c r="AJ28" s="13"/>
+      <c r="AK28" s="13"/>
+      <c r="AL28" s="14"/>
+      <c r="AO28" s="12"/>
+      <c r="AP28" s="13"/>
+      <c r="AQ28" s="13"/>
+      <c r="AR28" s="13"/>
+      <c r="AS28" s="13"/>
+      <c r="AT28" s="13"/>
+      <c r="AU28" s="13"/>
+      <c r="AV28" s="13"/>
+      <c r="AW28" s="13"/>
+      <c r="AX28" s="13"/>
+      <c r="AY28" s="13"/>
+      <c r="AZ28" s="13"/>
+      <c r="BA28" s="14"/>
+    </row>
+    <row r="29" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E29" s="2">
+        <v>9</v>
+      </c>
+      <c r="F29" s="2">
+        <v>99.816000000000003</v>
+      </c>
+      <c r="G29" s="2">
+        <v>100</v>
+      </c>
+      <c r="H29" s="2">
+        <v>99.981999999999999</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K29" s="2">
+        <v>8</v>
+      </c>
+      <c r="L29" s="2">
+        <v>99.775000000000006</v>
+      </c>
+      <c r="M29" s="2">
+        <v>100</v>
+      </c>
+      <c r="N29" s="2">
+        <v>99.974999999999994</v>
+      </c>
+      <c r="Q29" s="12"/>
+      <c r="R29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S29" s="2">
+        <v>8</v>
+      </c>
+      <c r="T29" s="2">
+        <v>99.754000000000005</v>
+      </c>
+      <c r="U29" s="13">
+        <v>8</v>
+      </c>
+      <c r="V29" s="2">
+        <v>99.997</v>
+      </c>
+      <c r="W29" s="13"/>
+      <c r="X29" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y29" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z29" s="2">
+        <v>99.825999999999993</v>
+      </c>
+      <c r="AA29" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB29" s="2">
+        <v>100</v>
+      </c>
+      <c r="AC29" s="13"/>
+      <c r="AD29" s="13"/>
+      <c r="AE29" s="13"/>
+      <c r="AF29" s="13"/>
+      <c r="AG29" s="13"/>
+      <c r="AH29" s="13"/>
+      <c r="AI29" s="13"/>
+      <c r="AJ29" s="13"/>
+      <c r="AK29" s="13"/>
+      <c r="AL29" s="14"/>
+      <c r="AO29" s="12"/>
+      <c r="AP29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="AQ29" s="5"/>
+      <c r="AR29" s="13"/>
+      <c r="AS29" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="AT29" s="5"/>
+      <c r="AU29" s="13"/>
+      <c r="AV29" s="13"/>
+      <c r="AW29" s="13"/>
+      <c r="AX29" s="13"/>
+      <c r="AY29" s="13"/>
+      <c r="AZ29" s="13"/>
+      <c r="BA29" s="14"/>
+    </row>
+    <row r="30" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q30" s="12"/>
+      <c r="R30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S30" s="2">
+        <v>10</v>
+      </c>
+      <c r="T30" s="2">
+        <v>99.816000000000003</v>
+      </c>
+      <c r="U30" s="2">
+        <v>10</v>
+      </c>
+      <c r="V30" s="2">
+        <v>100</v>
+      </c>
+      <c r="W30" s="13"/>
+      <c r="X30" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y30" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z30" s="2">
+        <v>99.775000000000006</v>
+      </c>
+      <c r="AA30" s="2">
+        <v>9</v>
+      </c>
+      <c r="AB30" s="2">
+        <v>100</v>
+      </c>
+      <c r="AC30" s="13"/>
+      <c r="AD30" s="13"/>
+      <c r="AE30" s="13"/>
+      <c r="AF30" s="13"/>
+      <c r="AG30" s="13"/>
+      <c r="AH30" s="13"/>
+      <c r="AI30" s="13"/>
+      <c r="AJ30" s="13"/>
+      <c r="AK30" s="13"/>
+      <c r="AL30" s="14"/>
+      <c r="AO30" s="12"/>
+      <c r="AP30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR30" s="13"/>
+      <c r="AS30" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU30" s="13"/>
+      <c r="AV30" s="13"/>
+      <c r="AW30" s="13"/>
+      <c r="AX30" s="13"/>
+      <c r="AY30" s="13"/>
+      <c r="AZ30" s="13"/>
+      <c r="BA30" s="14"/>
+    </row>
+    <row r="31" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q31" s="12"/>
+      <c r="R31" s="13"/>
+      <c r="S31" s="13"/>
+      <c r="T31" s="13"/>
+      <c r="U31" s="13"/>
+      <c r="V31" s="13"/>
+      <c r="W31" s="13"/>
+      <c r="X31" s="13"/>
+      <c r="Y31" s="13"/>
+      <c r="Z31" s="13"/>
+      <c r="AA31" s="13"/>
+      <c r="AB31" s="13"/>
+      <c r="AC31" s="13"/>
+      <c r="AD31" s="13"/>
+      <c r="AE31" s="13"/>
+      <c r="AF31" s="13"/>
+      <c r="AG31" s="13"/>
+      <c r="AH31" s="13"/>
+      <c r="AI31" s="13"/>
+      <c r="AJ31" s="13"/>
+      <c r="AK31" s="13"/>
+      <c r="AL31" s="14"/>
+      <c r="AO31" s="12"/>
+      <c r="AP31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ31" s="2"/>
+      <c r="AR31" s="13"/>
+      <c r="AS31" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT31" s="2"/>
+      <c r="AU31" s="13"/>
+      <c r="AV31" s="13"/>
+      <c r="AW31" s="13"/>
+      <c r="AX31" s="13"/>
+      <c r="AY31" s="13"/>
+      <c r="AZ31" s="13"/>
+      <c r="BA31" s="14"/>
+    </row>
+    <row r="32" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D32" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="7"/>
+      <c r="G32" s="7"/>
+      <c r="H32" s="8"/>
+      <c r="J32" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="K32" s="7"/>
+      <c r="L32" s="7"/>
+      <c r="M32" s="7"/>
+      <c r="N32" s="8"/>
+      <c r="Q32" s="12"/>
+      <c r="R32" s="13"/>
+      <c r="S32" s="13"/>
+      <c r="T32" s="13"/>
+      <c r="U32" s="13"/>
+      <c r="V32" s="13"/>
+      <c r="W32" s="13"/>
+      <c r="X32" s="13"/>
+      <c r="Y32" s="13"/>
+      <c r="Z32" s="13"/>
+      <c r="AA32" s="13"/>
+      <c r="AB32" s="13"/>
+      <c r="AC32" s="13"/>
+      <c r="AD32" s="13"/>
+      <c r="AE32" s="13"/>
+      <c r="AF32" s="13"/>
+      <c r="AG32" s="13"/>
+      <c r="AH32" s="13"/>
+      <c r="AI32" s="13"/>
+      <c r="AJ32" s="13"/>
+      <c r="AK32" s="13"/>
+      <c r="AL32" s="14"/>
+      <c r="AO32" s="12"/>
+      <c r="AP32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ32" s="2"/>
+      <c r="AR32" s="13"/>
+      <c r="AS32" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT32" s="2"/>
+      <c r="AU32" s="13"/>
+      <c r="AV32" s="13"/>
+      <c r="AW32" s="13"/>
+      <c r="AX32" s="13"/>
+      <c r="AY32" s="13"/>
+      <c r="AZ32" s="13"/>
+      <c r="BA32" s="14"/>
+    </row>
+    <row r="33" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D33" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G24" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="K24" s="3" t="s">
+      <c r="K33" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="L33" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="M24" s="3" t="s">
+      <c r="M33" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="3" t="s">
+      <c r="N33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="R24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V24" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X24" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y24" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB24" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="25" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D25" s="4" t="s">
+      <c r="Q33" s="12"/>
+      <c r="R33" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="8"/>
+      <c r="W33" s="13"/>
+      <c r="X33" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="8"/>
+      <c r="AC33" s="13"/>
+      <c r="AD33" s="13"/>
+      <c r="AE33" s="13"/>
+      <c r="AF33" s="13"/>
+      <c r="AG33" s="13"/>
+      <c r="AH33" s="13"/>
+      <c r="AI33" s="13"/>
+      <c r="AJ33" s="13"/>
+      <c r="AK33" s="13"/>
+      <c r="AL33" s="14"/>
+      <c r="AO33" s="12"/>
+      <c r="AP33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ33" s="2"/>
+      <c r="AR33" s="13"/>
+      <c r="AS33" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT33" s="2"/>
+      <c r="AU33" s="13"/>
+      <c r="AV33" s="13"/>
+      <c r="AW33" s="13"/>
+      <c r="AX33" s="13"/>
+      <c r="AY33" s="13"/>
+      <c r="AZ33" s="13"/>
+      <c r="BA33" s="14"/>
+    </row>
+    <row r="34" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D34" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="2">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2">
-        <v>98.71</v>
-      </c>
-      <c r="G25" s="2">
-        <v>99.188000000000002</v>
-      </c>
-      <c r="H25" s="2">
-        <v>99.128</v>
-      </c>
-      <c r="J25" s="4" t="s">
+      <c r="E34" s="2">
+        <v>10</v>
+      </c>
+      <c r="F34" s="2">
+        <v>99.385999999999996</v>
+      </c>
+      <c r="G34" s="2">
+        <v>99.701999999999998</v>
+      </c>
+      <c r="H34" s="2">
+        <v>99.67</v>
+      </c>
+      <c r="J34" s="4" t="s">
         <v>1</v>
-      </c>
-      <c r="K25" s="2">
-        <v>10</v>
-      </c>
-      <c r="L25" s="2">
-        <v>99.15</v>
-      </c>
-      <c r="M25" s="2">
-        <v>99.465999999999994</v>
-      </c>
-      <c r="N25" s="2">
-        <v>99.435000000000002</v>
-      </c>
-      <c r="R25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S25" s="2">
-        <v>8</v>
-      </c>
-      <c r="T25" s="2">
-        <v>98.71</v>
-      </c>
-      <c r="U25" s="2">
-        <v>8</v>
-      </c>
-      <c r="V25" s="2">
-        <v>99.188000000000002</v>
-      </c>
-      <c r="X25" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y25" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z25" s="2">
-        <v>99.15</v>
-      </c>
-      <c r="AA25" s="2">
-        <v>10</v>
-      </c>
-      <c r="AB25" s="2">
-        <v>99.465999999999994</v>
-      </c>
-    </row>
-    <row r="26" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D26" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E26" s="2">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2">
-        <v>99.754000000000005</v>
-      </c>
-      <c r="G26" s="2">
-        <v>99.997</v>
-      </c>
-      <c r="H26" s="2">
-        <v>99.966999999999999</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K26" s="2">
-        <v>10</v>
-      </c>
-      <c r="L26" s="2">
-        <v>99.825999999999993</v>
-      </c>
-      <c r="M26" s="2">
-        <v>100</v>
-      </c>
-      <c r="N26" s="2">
-        <v>99.983000000000004</v>
-      </c>
-      <c r="R26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S26" s="2">
-        <v>8</v>
-      </c>
-      <c r="T26" s="2">
-        <v>99.754000000000005</v>
-      </c>
-      <c r="U26" s="1">
-        <v>8</v>
-      </c>
-      <c r="V26" s="2">
-        <v>99.997</v>
-      </c>
-      <c r="X26" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y26" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z26" s="2">
-        <v>99.825999999999993</v>
-      </c>
-      <c r="AA26" s="2">
-        <v>10</v>
-      </c>
-      <c r="AB26" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2">
-        <v>9</v>
-      </c>
-      <c r="F27" s="2">
-        <v>99.816000000000003</v>
-      </c>
-      <c r="G27" s="2">
-        <v>100</v>
-      </c>
-      <c r="H27" s="2">
-        <v>99.981999999999999</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="K27" s="2">
-        <v>8</v>
-      </c>
-      <c r="L27" s="2">
-        <v>99.775000000000006</v>
-      </c>
-      <c r="M27" s="2">
-        <v>100</v>
-      </c>
-      <c r="N27" s="2">
-        <v>99.974999999999994</v>
-      </c>
-      <c r="R27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S27" s="2">
-        <v>10</v>
-      </c>
-      <c r="T27" s="2">
-        <v>99.816000000000003</v>
-      </c>
-      <c r="U27" s="2">
-        <v>10</v>
-      </c>
-      <c r="V27" s="2">
-        <v>100</v>
-      </c>
-      <c r="X27" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="Y27" s="2">
-        <v>9</v>
-      </c>
-      <c r="Z27" s="2">
-        <v>99.775000000000006</v>
-      </c>
-      <c r="AA27" s="2">
-        <v>9</v>
-      </c>
-      <c r="AB27" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="30" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
-      <c r="H30" s="8"/>
-      <c r="J30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="K30" s="7"/>
-      <c r="L30" s="7"/>
-      <c r="M30" s="7"/>
-      <c r="N30" s="8"/>
-      <c r="R30" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="S30" s="7"/>
-      <c r="T30" s="7"/>
-      <c r="U30" s="7"/>
-      <c r="V30" s="8"/>
-      <c r="X30" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Y30" s="7"/>
-      <c r="Z30" s="7"/>
-      <c r="AA30" s="7"/>
-      <c r="AB30" s="8"/>
-    </row>
-    <row r="31" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="K31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="L31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="M31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="N31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V31" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="X31" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y31" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="Z31" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="AA31" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="AB31" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32" s="2">
-        <v>10</v>
-      </c>
-      <c r="F32" s="2">
-        <v>99.385999999999996</v>
-      </c>
-      <c r="G32" s="2">
-        <v>99.701999999999998</v>
-      </c>
-      <c r="H32" s="2">
-        <v>99.67</v>
-      </c>
-      <c r="J32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K32" s="2">
-        <v>9</v>
-      </c>
-      <c r="L32" s="2">
-        <v>99.528999999999996</v>
-      </c>
-      <c r="M32" s="2">
-        <v>99.763999999999996</v>
-      </c>
-      <c r="N32" s="2">
-        <v>99.738</v>
-      </c>
-      <c r="R32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S32" s="2">
-        <v>10</v>
-      </c>
-      <c r="T32" s="2">
-        <v>99.385999999999996</v>
-      </c>
-      <c r="U32" s="1">
-        <v>10</v>
-      </c>
-      <c r="V32" s="2">
-        <v>99.701999999999998</v>
-      </c>
-      <c r="X32" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y32" s="2">
-        <v>9</v>
-      </c>
-      <c r="Z32" s="2">
-        <v>99.528999999999996</v>
-      </c>
-      <c r="AA32" s="2">
-        <v>9</v>
-      </c>
-      <c r="AB32" s="2">
-        <v>99.763999999999996</v>
-      </c>
-    </row>
-    <row r="33" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E33" s="2">
-        <v>10</v>
-      </c>
-      <c r="F33" s="2">
-        <v>99.703000000000003</v>
-      </c>
-      <c r="G33" s="2">
-        <v>100</v>
-      </c>
-      <c r="H33" s="2">
-        <v>99.97</v>
-      </c>
-      <c r="J33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K33" s="2">
-        <v>10</v>
-      </c>
-      <c r="L33" s="2">
-        <v>99.754000000000005</v>
-      </c>
-      <c r="M33" s="2">
-        <v>99.997</v>
-      </c>
-      <c r="N33" s="2">
-        <v>99.971999999999994</v>
-      </c>
-      <c r="R33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S33" s="2">
-        <v>9</v>
-      </c>
-      <c r="T33" s="2">
-        <v>99.724000000000004</v>
-      </c>
-      <c r="U33" s="2">
-        <v>9</v>
-      </c>
-      <c r="V33" s="2">
-        <v>100</v>
-      </c>
-      <c r="X33" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y33" s="2">
-        <v>10</v>
-      </c>
-      <c r="Z33" s="2">
-        <v>99.754000000000005</v>
-      </c>
-      <c r="AA33" s="2">
-        <v>10</v>
-      </c>
-      <c r="AB33" s="2">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="34" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D34" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="2">
-        <v>9</v>
-      </c>
-      <c r="F34" s="2">
-        <v>99.775000000000006</v>
-      </c>
-      <c r="G34" s="2">
-        <v>100</v>
-      </c>
-      <c r="H34" s="2">
-        <v>99.977000000000004</v>
-      </c>
-      <c r="J34" s="4" t="s">
-        <v>3</v>
       </c>
       <c r="K34" s="2">
         <v>9</v>
       </c>
       <c r="L34" s="2">
+        <v>99.528999999999996</v>
+      </c>
+      <c r="M34" s="2">
+        <v>99.763999999999996</v>
+      </c>
+      <c r="N34" s="2">
+        <v>99.738</v>
+      </c>
+      <c r="Q34" s="12"/>
+      <c r="R34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="W34" s="13"/>
+      <c r="X34" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Z34" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB34" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="AC34" s="13"/>
+      <c r="AD34" s="13"/>
+      <c r="AE34" s="13"/>
+      <c r="AF34" s="13"/>
+      <c r="AG34" s="13"/>
+      <c r="AH34" s="13"/>
+      <c r="AI34" s="13"/>
+      <c r="AJ34" s="13"/>
+      <c r="AK34" s="13"/>
+      <c r="AL34" s="14"/>
+      <c r="AO34" s="12"/>
+      <c r="AP34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ34" s="2" t="e">
+        <f>AVERAGE(AQ31:AQ33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR34" s="13"/>
+      <c r="AS34" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT34" s="2" t="e">
+        <f>AVERAGE(AT31:AT33)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU34" s="13"/>
+      <c r="AV34" s="13"/>
+      <c r="AW34" s="13"/>
+      <c r="AX34" s="13"/>
+      <c r="AY34" s="13"/>
+      <c r="AZ34" s="13"/>
+      <c r="BA34" s="14"/>
+    </row>
+    <row r="35" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" s="2">
+        <v>10</v>
+      </c>
+      <c r="F35" s="2">
+        <v>99.703000000000003</v>
+      </c>
+      <c r="G35" s="2">
+        <v>100</v>
+      </c>
+      <c r="H35" s="2">
+        <v>99.97</v>
+      </c>
+      <c r="J35" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K35" s="2">
+        <v>10</v>
+      </c>
+      <c r="L35" s="2">
+        <v>99.754000000000005</v>
+      </c>
+      <c r="M35" s="2">
+        <v>99.997</v>
+      </c>
+      <c r="N35" s="2">
+        <v>99.971999999999994</v>
+      </c>
+      <c r="Q35" s="12"/>
+      <c r="R35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S35" s="2">
+        <v>10</v>
+      </c>
+      <c r="T35" s="2">
+        <v>99.385999999999996</v>
+      </c>
+      <c r="U35" s="13">
+        <v>10</v>
+      </c>
+      <c r="V35" s="2">
+        <v>99.701999999999998</v>
+      </c>
+      <c r="W35" s="13"/>
+      <c r="X35" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>9</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>99.528999999999996</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>9</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>99.763999999999996</v>
+      </c>
+      <c r="AC35" s="13"/>
+      <c r="AD35" s="13"/>
+      <c r="AE35" s="13"/>
+      <c r="AF35" s="13"/>
+      <c r="AG35" s="13"/>
+      <c r="AH35" s="13"/>
+      <c r="AI35" s="13"/>
+      <c r="AJ35" s="13"/>
+      <c r="AK35" s="13"/>
+      <c r="AL35" s="14"/>
+      <c r="AO35" s="12"/>
+      <c r="AP35" s="13"/>
+      <c r="AQ35" s="13"/>
+      <c r="AR35" s="13"/>
+      <c r="AS35" s="13"/>
+      <c r="AT35" s="13"/>
+      <c r="AU35" s="13"/>
+      <c r="AV35" s="13"/>
+      <c r="AW35" s="13"/>
+      <c r="AX35" s="13"/>
+      <c r="AY35" s="13"/>
+      <c r="AZ35" s="13"/>
+      <c r="BA35" s="14"/>
+    </row>
+    <row r="36" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E36" s="2">
+        <v>9</v>
+      </c>
+      <c r="F36" s="2">
+        <v>99.775000000000006</v>
+      </c>
+      <c r="G36" s="2">
+        <v>100</v>
+      </c>
+      <c r="H36" s="2">
+        <v>99.977000000000004</v>
+      </c>
+      <c r="J36" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K36" s="2">
+        <v>9</v>
+      </c>
+      <c r="L36" s="2">
         <v>99.733999999999995</v>
       </c>
-      <c r="M34" s="2">
+      <c r="M36" s="2">
         <v>100</v>
       </c>
-      <c r="N34" s="2">
+      <c r="N36" s="2">
         <v>99.972999999999999</v>
       </c>
-      <c r="R34" s="4" t="s">
+      <c r="Q36" s="12"/>
+      <c r="R36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S36" s="2">
+        <v>9</v>
+      </c>
+      <c r="T36" s="2">
+        <v>99.724000000000004</v>
+      </c>
+      <c r="U36" s="2">
+        <v>9</v>
+      </c>
+      <c r="V36" s="2">
+        <v>100</v>
+      </c>
+      <c r="W36" s="13"/>
+      <c r="X36" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y36" s="2">
+        <v>10</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>99.754000000000005</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>10</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>100</v>
+      </c>
+      <c r="AC36" s="13"/>
+      <c r="AD36" s="13"/>
+      <c r="AE36" s="13"/>
+      <c r="AF36" s="13"/>
+      <c r="AG36" s="13"/>
+      <c r="AH36" s="13"/>
+      <c r="AI36" s="13"/>
+      <c r="AJ36" s="13"/>
+      <c r="AK36" s="13"/>
+      <c r="AL36" s="14"/>
+      <c r="AO36" s="12"/>
+      <c r="AP36" s="13"/>
+      <c r="AQ36" s="13"/>
+      <c r="AR36" s="13"/>
+      <c r="AS36" s="13"/>
+      <c r="AT36" s="13"/>
+      <c r="AU36" s="13"/>
+      <c r="AV36" s="13"/>
+      <c r="AW36" s="13"/>
+      <c r="AX36" s="13"/>
+      <c r="AY36" s="13"/>
+      <c r="AZ36" s="13"/>
+      <c r="BA36" s="14"/>
+    </row>
+    <row r="37" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q37" s="12"/>
+      <c r="R37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="S34" s="2">
+      <c r="S37" s="2">
         <v>10</v>
       </c>
-      <c r="T34" s="2">
+      <c r="T37" s="2">
         <v>99.775000000000006</v>
       </c>
-      <c r="U34" s="2">
+      <c r="U37" s="2">
         <v>10</v>
       </c>
-      <c r="V34" s="2">
+      <c r="V37" s="2">
         <v>100</v>
       </c>
-      <c r="X34" s="4" t="s">
+      <c r="W37" s="13"/>
+      <c r="X37" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="Y34" s="2">
+      <c r="Y37" s="2">
         <v>10</v>
       </c>
-      <c r="Z34" s="2">
+      <c r="Z37" s="2">
         <v>99.733999999999995</v>
       </c>
-      <c r="AA34" s="2">
+      <c r="AA37" s="2">
         <v>10</v>
       </c>
-      <c r="AB34" s="2">
+      <c r="AB37" s="2">
         <v>100</v>
       </c>
-    </row>
-    <row r="35" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="AA35" s="1" t="s">
+      <c r="AC37" s="13"/>
+      <c r="AD37" s="13"/>
+      <c r="AE37" s="13"/>
+      <c r="AF37" s="13"/>
+      <c r="AG37" s="13"/>
+      <c r="AH37" s="13"/>
+      <c r="AI37" s="13"/>
+      <c r="AJ37" s="13"/>
+      <c r="AK37" s="13"/>
+      <c r="AL37" s="14"/>
+      <c r="AO37" s="12"/>
+      <c r="AP37" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="AQ37" s="5"/>
+      <c r="AR37" s="13"/>
+      <c r="AS37" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="AT37" s="5"/>
+      <c r="AU37" s="13"/>
+      <c r="AV37" s="13"/>
+      <c r="AW37" s="13"/>
+      <c r="AX37" s="13"/>
+      <c r="AY37" s="13"/>
+      <c r="AZ37" s="13"/>
+      <c r="BA37" s="14"/>
+    </row>
+    <row r="38" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q38" s="12"/>
+      <c r="R38" s="13"/>
+      <c r="S38" s="13"/>
+      <c r="T38" s="13"/>
+      <c r="U38" s="13"/>
+      <c r="V38" s="13"/>
+      <c r="W38" s="13"/>
+      <c r="X38" s="13"/>
+      <c r="Y38" s="13"/>
+      <c r="Z38" s="13"/>
+      <c r="AA38" s="13" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D37" s="6" t="s">
+      <c r="AB38" s="13"/>
+      <c r="AC38" s="13"/>
+      <c r="AD38" s="13"/>
+      <c r="AE38" s="13"/>
+      <c r="AF38" s="13"/>
+      <c r="AG38" s="13"/>
+      <c r="AH38" s="13"/>
+      <c r="AI38" s="13"/>
+      <c r="AJ38" s="13"/>
+      <c r="AK38" s="13"/>
+      <c r="AL38" s="14"/>
+      <c r="AO38" s="12"/>
+      <c r="AP38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AQ38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR38" s="13"/>
+      <c r="AS38" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="AT38" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU38" s="13"/>
+      <c r="AV38" s="13"/>
+      <c r="AW38" s="13"/>
+      <c r="AX38" s="13"/>
+      <c r="AY38" s="13"/>
+      <c r="AZ38" s="13"/>
+      <c r="BA38" s="14"/>
+    </row>
+    <row r="39" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D39" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="E37" s="7"/>
-      <c r="F37" s="7"/>
-      <c r="G37" s="7"/>
-      <c r="H37" s="8"/>
-      <c r="R37" s="6" t="s">
+      <c r="E39" s="7"/>
+      <c r="F39" s="7"/>
+      <c r="G39" s="7"/>
+      <c r="H39" s="8"/>
+      <c r="Q39" s="12"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
+      <c r="T39" s="13"/>
+      <c r="U39" s="13"/>
+      <c r="V39" s="13"/>
+      <c r="W39" s="13"/>
+      <c r="X39" s="13"/>
+      <c r="Y39" s="13"/>
+      <c r="Z39" s="13"/>
+      <c r="AA39" s="13"/>
+      <c r="AB39" s="13"/>
+      <c r="AC39" s="13"/>
+      <c r="AD39" s="13"/>
+      <c r="AE39" s="13"/>
+      <c r="AF39" s="13"/>
+      <c r="AG39" s="13"/>
+      <c r="AH39" s="13"/>
+      <c r="AI39" s="13"/>
+      <c r="AJ39" s="13"/>
+      <c r="AK39" s="13"/>
+      <c r="AL39" s="14"/>
+      <c r="AO39" s="12"/>
+      <c r="AP39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AQ39" s="2"/>
+      <c r="AR39" s="13"/>
+      <c r="AS39" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AT39" s="2"/>
+      <c r="AU39" s="13"/>
+      <c r="AV39" s="13"/>
+      <c r="AW39" s="13"/>
+      <c r="AX39" s="13"/>
+      <c r="AY39" s="13"/>
+      <c r="AZ39" s="13"/>
+      <c r="BA39" s="14"/>
+    </row>
+    <row r="40" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D40" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F40" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q40" s="12"/>
+      <c r="R40" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="S37" s="7"/>
-      <c r="T37" s="7"/>
-      <c r="U37" s="7"/>
-      <c r="V37" s="8"/>
-    </row>
-    <row r="38" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D38" s="3" t="s">
+      <c r="S40" s="7"/>
+      <c r="T40" s="7"/>
+      <c r="U40" s="7"/>
+      <c r="V40" s="8"/>
+      <c r="W40" s="13"/>
+      <c r="X40" s="13"/>
+      <c r="Y40" s="13"/>
+      <c r="Z40" s="13"/>
+      <c r="AA40" s="13"/>
+      <c r="AB40" s="13"/>
+      <c r="AC40" s="13"/>
+      <c r="AD40" s="13"/>
+      <c r="AE40" s="13"/>
+      <c r="AF40" s="13"/>
+      <c r="AG40" s="13"/>
+      <c r="AH40" s="13"/>
+      <c r="AI40" s="13"/>
+      <c r="AJ40" s="13"/>
+      <c r="AK40" s="13"/>
+      <c r="AL40" s="14"/>
+      <c r="AO40" s="12"/>
+      <c r="AP40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AQ40" s="2"/>
+      <c r="AR40" s="13"/>
+      <c r="AS40" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AT40" s="2"/>
+      <c r="AU40" s="13"/>
+      <c r="AV40" s="13"/>
+      <c r="AW40" s="13"/>
+      <c r="AX40" s="13"/>
+      <c r="AY40" s="13"/>
+      <c r="AZ40" s="13"/>
+      <c r="BA40" s="14"/>
+    </row>
+    <row r="41" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D41" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41" s="2">
+        <v>10</v>
+      </c>
+      <c r="F41" s="2">
+        <v>98.525000000000006</v>
+      </c>
+      <c r="G41" s="2">
+        <v>98.804000000000002</v>
+      </c>
+      <c r="H41" s="2">
+        <v>98.775999999999996</v>
+      </c>
+      <c r="Q41" s="12"/>
+      <c r="R41" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="3" t="s">
+      <c r="S41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="T41" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G38" s="3" t="s">
+      <c r="U41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="V41" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H38" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="R38" s="3" t="s">
+      <c r="W41" s="13"/>
+      <c r="X41" s="13"/>
+      <c r="Y41" s="13"/>
+      <c r="Z41" s="13"/>
+      <c r="AA41" s="13"/>
+      <c r="AB41" s="13"/>
+      <c r="AC41" s="13"/>
+      <c r="AD41" s="13"/>
+      <c r="AE41" s="13"/>
+      <c r="AF41" s="13"/>
+      <c r="AG41" s="13"/>
+      <c r="AH41" s="13"/>
+      <c r="AI41" s="13"/>
+      <c r="AJ41" s="13"/>
+      <c r="AK41" s="13"/>
+      <c r="AL41" s="14"/>
+      <c r="AO41" s="12"/>
+      <c r="AP41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AQ41" s="2"/>
+      <c r="AR41" s="13"/>
+      <c r="AS41" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT41" s="2"/>
+      <c r="AU41" s="13"/>
+      <c r="AV41" s="13"/>
+      <c r="AW41" s="13"/>
+      <c r="AX41" s="13"/>
+      <c r="AY41" s="13"/>
+      <c r="AZ41" s="13"/>
+      <c r="BA41" s="14"/>
+    </row>
+    <row r="42" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D42" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E42" s="2">
+        <v>10</v>
+      </c>
+      <c r="F42" s="2">
+        <v>98.832999999999998</v>
+      </c>
+      <c r="G42" s="2">
+        <v>99.106999999999999</v>
+      </c>
+      <c r="H42" s="2">
+        <v>99.078999999999994</v>
+      </c>
+      <c r="Q42" s="12"/>
+      <c r="R42" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S42" s="2">
+        <v>10</v>
+      </c>
+      <c r="T42" s="2">
+        <v>98.525000000000006</v>
+      </c>
+      <c r="U42" s="2">
+        <v>10</v>
+      </c>
+      <c r="V42" s="2">
+        <v>98.804000000000002</v>
+      </c>
+      <c r="W42" s="13"/>
+      <c r="X42" s="13"/>
+      <c r="Y42" s="13"/>
+      <c r="Z42" s="13"/>
+      <c r="AA42" s="13"/>
+      <c r="AB42" s="13"/>
+      <c r="AC42" s="13"/>
+      <c r="AD42" s="13"/>
+      <c r="AE42" s="13"/>
+      <c r="AF42" s="13"/>
+      <c r="AG42" s="13"/>
+      <c r="AH42" s="13"/>
+      <c r="AI42" s="13"/>
+      <c r="AJ42" s="13"/>
+      <c r="AK42" s="13"/>
+      <c r="AL42" s="14"/>
+      <c r="AO42" s="12"/>
+      <c r="AP42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ42" s="2" t="e">
+        <f>AVERAGE(AQ39:AQ41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AR42" s="13"/>
+      <c r="AS42" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AT42" s="2" t="e">
+        <f>AVERAGE(AT39:AT41)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AU42" s="13"/>
+      <c r="AV42" s="13"/>
+      <c r="AW42" s="13"/>
+      <c r="AX42" s="13"/>
+      <c r="AY42" s="13"/>
+      <c r="AZ42" s="13"/>
+      <c r="BA42" s="14"/>
+    </row>
+    <row r="43" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="D43" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E43" s="2">
+        <v>7</v>
+      </c>
+      <c r="F43" s="2">
+        <v>99.099000000000004</v>
+      </c>
+      <c r="G43" s="2">
+        <v>99.447000000000003</v>
+      </c>
+      <c r="H43" s="2">
+        <v>99.397000000000006</v>
+      </c>
+      <c r="Q43" s="12"/>
+      <c r="R43" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S43" s="2">
+        <v>10</v>
+      </c>
+      <c r="T43" s="2">
+        <v>98.832999999999998</v>
+      </c>
+      <c r="U43" s="2">
+        <v>10</v>
+      </c>
+      <c r="V43" s="2">
+        <v>99.106999999999999</v>
+      </c>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Y43" s="13"/>
+      <c r="Z43" s="13"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
+      <c r="AC43" s="13"/>
+      <c r="AD43" s="13"/>
+      <c r="AE43" s="13"/>
+      <c r="AF43" s="13"/>
+      <c r="AG43" s="13"/>
+      <c r="AH43" s="13"/>
+      <c r="AI43" s="13"/>
+      <c r="AJ43" s="13"/>
+      <c r="AK43" s="13"/>
+      <c r="AL43" s="14"/>
+      <c r="AO43" s="12"/>
+      <c r="AP43" s="13"/>
+      <c r="AQ43" s="13"/>
+      <c r="AR43" s="13"/>
+      <c r="AS43" s="13"/>
+      <c r="AT43" s="13"/>
+      <c r="AU43" s="13"/>
+      <c r="AV43" s="13"/>
+      <c r="AW43" s="13"/>
+      <c r="AX43" s="13"/>
+      <c r="AY43" s="13"/>
+      <c r="AZ43" s="13"/>
+      <c r="BA43" s="14"/>
+    </row>
+    <row r="44" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q44" s="12"/>
+      <c r="R44" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="S44" s="2">
+        <v>9</v>
+      </c>
+      <c r="T44" s="2">
+        <v>99.108999999999995</v>
+      </c>
+      <c r="U44" s="2">
+        <v>7</v>
+      </c>
+      <c r="V44" s="2">
+        <v>99.447000000000003</v>
+      </c>
+      <c r="W44" s="13"/>
+      <c r="X44" s="13"/>
+      <c r="Y44" s="13"/>
+      <c r="Z44" s="13"/>
+      <c r="AA44" s="13"/>
+      <c r="AB44" s="13"/>
+      <c r="AC44" s="13"/>
+      <c r="AD44" s="13"/>
+      <c r="AE44" s="13"/>
+      <c r="AF44" s="13"/>
+      <c r="AG44" s="13"/>
+      <c r="AH44" s="13"/>
+      <c r="AI44" s="13"/>
+      <c r="AJ44" s="13"/>
+      <c r="AK44" s="13"/>
+      <c r="AL44" s="14"/>
+      <c r="AO44" s="12"/>
+      <c r="AP44" s="13"/>
+      <c r="AQ44" s="13"/>
+      <c r="AR44" s="13"/>
+      <c r="AS44" s="13"/>
+      <c r="AT44" s="13"/>
+      <c r="AU44" s="13"/>
+      <c r="AV44" s="13"/>
+      <c r="AW44" s="13"/>
+      <c r="AX44" s="13"/>
+      <c r="AY44" s="13"/>
+      <c r="AZ44" s="13"/>
+      <c r="BA44" s="14"/>
+    </row>
+    <row r="45" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q45" s="12"/>
+      <c r="R45" s="13"/>
+      <c r="S45" s="13"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+      <c r="V45" s="13"/>
+      <c r="W45" s="13"/>
+      <c r="X45" s="13"/>
+      <c r="Y45" s="13"/>
+      <c r="Z45" s="13"/>
+      <c r="AA45" s="13"/>
+      <c r="AB45" s="13"/>
+      <c r="AC45" s="13"/>
+      <c r="AD45" s="13"/>
+      <c r="AE45" s="13"/>
+      <c r="AF45" s="13"/>
+      <c r="AG45" s="13"/>
+      <c r="AH45" s="13"/>
+      <c r="AI45" s="13"/>
+      <c r="AJ45" s="13"/>
+      <c r="AK45" s="13"/>
+      <c r="AL45" s="14"/>
+      <c r="AO45" s="12"/>
+      <c r="AP45" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="AQ45" s="5"/>
+      <c r="AR45" s="13"/>
+      <c r="AS45" s="13"/>
+      <c r="AT45" s="13"/>
+      <c r="AU45" s="13"/>
+      <c r="AV45" s="13"/>
+      <c r="AW45" s="13"/>
+      <c r="AX45" s="13"/>
+      <c r="AY45" s="13"/>
+      <c r="AZ45" s="13"/>
+      <c r="BA45" s="14"/>
+    </row>
+    <row r="46" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q46" s="12"/>
+      <c r="R46" s="13"/>
+      <c r="S46" s="13"/>
+      <c r="T46" s="13"/>
+      <c r="U46" s="13"/>
+      <c r="V46" s="13"/>
+      <c r="W46" s="13"/>
+      <c r="X46" s="13"/>
+      <c r="Y46" s="13"/>
+      <c r="Z46" s="13"/>
+      <c r="AA46" s="13"/>
+      <c r="AB46" s="13"/>
+      <c r="AC46" s="13"/>
+      <c r="AD46" s="13"/>
+      <c r="AE46" s="13"/>
+      <c r="AF46" s="13"/>
+      <c r="AG46" s="13"/>
+      <c r="AH46" s="13"/>
+      <c r="AI46" s="13"/>
+      <c r="AJ46" s="13"/>
+      <c r="AK46" s="13"/>
+      <c r="AL46" s="14"/>
+      <c r="AO46" s="12"/>
+      <c r="AP46" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="S38" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="T38" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="U38" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="V38" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="39" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D39" s="4" t="s">
+      <c r="AQ46" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="AR46" s="13"/>
+      <c r="AS46" s="13"/>
+      <c r="AT46" s="13"/>
+      <c r="AU46" s="13"/>
+      <c r="AV46" s="13"/>
+      <c r="AW46" s="13"/>
+      <c r="AX46" s="13"/>
+      <c r="AY46" s="13"/>
+      <c r="AZ46" s="13"/>
+      <c r="BA46" s="14"/>
+    </row>
+    <row r="47" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q47" s="12"/>
+      <c r="R47" s="13"/>
+      <c r="S47" s="13"/>
+      <c r="T47" s="13"/>
+      <c r="U47" s="13"/>
+      <c r="V47" s="13"/>
+      <c r="W47" s="13"/>
+      <c r="X47" s="13"/>
+      <c r="Y47" s="13"/>
+      <c r="Z47" s="13"/>
+      <c r="AA47" s="13"/>
+      <c r="AB47" s="13"/>
+      <c r="AC47" s="13"/>
+      <c r="AD47" s="13"/>
+      <c r="AE47" s="13"/>
+      <c r="AF47" s="13"/>
+      <c r="AG47" s="13"/>
+      <c r="AH47" s="13"/>
+      <c r="AI47" s="13"/>
+      <c r="AJ47" s="13"/>
+      <c r="AK47" s="13"/>
+      <c r="AL47" s="14"/>
+      <c r="AO47" s="12"/>
+      <c r="AP47" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E39" s="2">
-        <v>10</v>
-      </c>
-      <c r="F39" s="2">
-        <v>98.525000000000006</v>
-      </c>
-      <c r="G39" s="2">
-        <v>98.804000000000002</v>
-      </c>
-      <c r="H39" s="2">
-        <v>98.775999999999996</v>
-      </c>
-      <c r="R39" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="S39" s="2">
-        <v>10</v>
-      </c>
-      <c r="T39" s="2">
-        <v>98.525000000000006</v>
-      </c>
-      <c r="U39" s="2">
-        <v>10</v>
-      </c>
-      <c r="V39" s="2">
-        <v>98.804000000000002</v>
-      </c>
-    </row>
-    <row r="40" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D40" s="4" t="s">
+      <c r="AQ47" s="2">
+        <v>8.3231999999999999</v>
+      </c>
+      <c r="AR47" s="13"/>
+      <c r="AS47" s="13"/>
+      <c r="AT47" s="13"/>
+      <c r="AU47" s="13"/>
+      <c r="AV47" s="13"/>
+      <c r="AW47" s="13"/>
+      <c r="AX47" s="13"/>
+      <c r="AY47" s="13"/>
+      <c r="AZ47" s="13"/>
+      <c r="BA47" s="14"/>
+    </row>
+    <row r="48" spans="4:53" x14ac:dyDescent="0.2">
+      <c r="Q48" s="12"/>
+      <c r="R48" s="13"/>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+      <c r="V48" s="13"/>
+      <c r="W48" s="13"/>
+      <c r="X48" s="13"/>
+      <c r="Y48" s="13"/>
+      <c r="Z48" s="13"/>
+      <c r="AA48" s="13"/>
+      <c r="AB48" s="13"/>
+      <c r="AC48" s="13"/>
+      <c r="AD48" s="13"/>
+      <c r="AE48" s="13"/>
+      <c r="AF48" s="13"/>
+      <c r="AG48" s="13"/>
+      <c r="AH48" s="13"/>
+      <c r="AI48" s="13"/>
+      <c r="AJ48" s="13"/>
+      <c r="AK48" s="13"/>
+      <c r="AL48" s="14"/>
+      <c r="AO48" s="12"/>
+      <c r="AP48" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E40" s="2">
-        <v>10</v>
-      </c>
-      <c r="F40" s="2">
-        <v>98.832999999999998</v>
-      </c>
-      <c r="G40" s="2">
-        <v>99.106999999999999</v>
-      </c>
-      <c r="H40" s="2">
-        <v>99.078999999999994</v>
-      </c>
-      <c r="R40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="S40" s="2">
-        <v>10</v>
-      </c>
-      <c r="T40" s="2">
-        <v>98.832999999999998</v>
-      </c>
-      <c r="U40" s="2">
-        <v>10</v>
-      </c>
-      <c r="V40" s="2">
-        <v>99.106999999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="4:28" x14ac:dyDescent="0.2">
-      <c r="D41" s="4" t="s">
+      <c r="AQ48" s="2">
+        <v>33.345100000000002</v>
+      </c>
+      <c r="AR48" s="13"/>
+      <c r="AS48" s="13"/>
+      <c r="AT48" s="13"/>
+      <c r="AU48" s="13"/>
+      <c r="AV48" s="13"/>
+      <c r="AW48" s="13"/>
+      <c r="AX48" s="13"/>
+      <c r="AY48" s="13"/>
+      <c r="AZ48" s="13"/>
+      <c r="BA48" s="14"/>
+    </row>
+    <row r="49" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="Q49" s="12"/>
+      <c r="R49" s="13"/>
+      <c r="S49" s="13"/>
+      <c r="T49" s="13"/>
+      <c r="U49" s="13"/>
+      <c r="V49" s="13"/>
+      <c r="W49" s="13"/>
+      <c r="X49" s="13"/>
+      <c r="Y49" s="13"/>
+      <c r="Z49" s="13"/>
+      <c r="AA49" s="13"/>
+      <c r="AB49" s="13"/>
+      <c r="AC49" s="13"/>
+      <c r="AD49" s="13"/>
+      <c r="AE49" s="13"/>
+      <c r="AF49" s="13"/>
+      <c r="AG49" s="13"/>
+      <c r="AH49" s="13"/>
+      <c r="AI49" s="13"/>
+      <c r="AJ49" s="13"/>
+      <c r="AK49" s="13"/>
+      <c r="AL49" s="14"/>
+      <c r="AO49" s="12"/>
+      <c r="AP49" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E41" s="2">
-        <v>7</v>
-      </c>
-      <c r="F41" s="2">
-        <v>99.099000000000004</v>
-      </c>
-      <c r="G41" s="2">
-        <v>99.447000000000003</v>
-      </c>
-      <c r="H41" s="2">
-        <v>99.397000000000006</v>
-      </c>
-      <c r="R41" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="S41" s="2">
-        <v>9</v>
-      </c>
-      <c r="T41" s="2">
-        <v>99.108999999999995</v>
-      </c>
-      <c r="U41" s="2">
-        <v>7</v>
-      </c>
-      <c r="V41" s="2">
-        <v>99.447000000000003</v>
-      </c>
+      <c r="AQ49" s="2">
+        <v>101.1771</v>
+      </c>
+      <c r="AR49" s="13"/>
+      <c r="AS49" s="13"/>
+      <c r="AT49" s="13"/>
+      <c r="AU49" s="13"/>
+      <c r="AV49" s="13"/>
+      <c r="AW49" s="13"/>
+      <c r="AX49" s="13"/>
+      <c r="AY49" s="13"/>
+      <c r="AZ49" s="13"/>
+      <c r="BA49" s="14"/>
+    </row>
+    <row r="50" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="Q50" s="12"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
+      <c r="T50" s="13"/>
+      <c r="U50" s="13"/>
+      <c r="V50" s="13"/>
+      <c r="W50" s="13"/>
+      <c r="X50" s="13"/>
+      <c r="Y50" s="13"/>
+      <c r="Z50" s="13"/>
+      <c r="AA50" s="13"/>
+      <c r="AB50" s="13"/>
+      <c r="AC50" s="13"/>
+      <c r="AD50" s="13"/>
+      <c r="AE50" s="13"/>
+      <c r="AF50" s="13"/>
+      <c r="AG50" s="13"/>
+      <c r="AH50" s="13"/>
+      <c r="AI50" s="13"/>
+      <c r="AJ50" s="13"/>
+      <c r="AK50" s="13"/>
+      <c r="AL50" s="14"/>
+      <c r="AO50" s="12"/>
+      <c r="AP50" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="AQ50" s="2">
+        <f>AVERAGE(AQ47:AQ49)</f>
+        <v>47.615133333333326</v>
+      </c>
+      <c r="AR50" s="13"/>
+      <c r="AS50" s="13"/>
+      <c r="AT50" s="13"/>
+      <c r="AU50" s="13"/>
+      <c r="AV50" s="13"/>
+      <c r="AW50" s="13"/>
+      <c r="AX50" s="13"/>
+      <c r="AY50" s="13"/>
+      <c r="AZ50" s="13"/>
+      <c r="BA50" s="14"/>
+    </row>
+    <row r="51" spans="17:53" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="Q51" s="15"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
+      <c r="W51" s="16"/>
+      <c r="X51" s="16"/>
+      <c r="Y51" s="16"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="16"/>
+      <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="16"/>
+      <c r="AH51" s="16"/>
+      <c r="AI51" s="16"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="17"/>
+      <c r="AO51" s="15"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="16"/>
+      <c r="AR51" s="16"/>
+      <c r="AS51" s="16"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="16"/>
+      <c r="AW51" s="16"/>
+      <c r="AX51" s="16"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="17"/>
+    </row>
+    <row r="52" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP52" s="13"/>
+    </row>
+    <row r="53" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP53" s="13"/>
+    </row>
+    <row r="54" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP54" s="13"/>
+    </row>
+    <row r="55" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP55" s="13"/>
+    </row>
+    <row r="56" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP56" s="13"/>
+    </row>
+    <row r="57" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP57" s="13"/>
+    </row>
+    <row r="58" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP58" s="13"/>
+    </row>
+    <row r="59" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP59" s="13"/>
+    </row>
+    <row r="60" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP60" s="13"/>
+    </row>
+    <row r="61" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP61" s="13"/>
+    </row>
+    <row r="62" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP62" s="13"/>
+    </row>
+    <row r="63" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP63" s="13"/>
+    </row>
+    <row r="64" spans="17:53" x14ac:dyDescent="0.2">
+      <c r="AP64" s="13"/>
+    </row>
+    <row r="65" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP65" s="13"/>
+    </row>
+    <row r="66" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP66" s="13"/>
+    </row>
+    <row r="67" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP67" s="13"/>
+    </row>
+    <row r="68" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP68" s="13"/>
+    </row>
+    <row r="69" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP69" s="13"/>
+    </row>
+    <row r="70" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP70" s="13"/>
+    </row>
+    <row r="71" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AP71" s="13"/>
+    </row>
+    <row r="78" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AQ78" s="13"/>
+      <c r="AR78" s="13"/>
+      <c r="AS78" s="13"/>
+      <c r="AT78" s="13"/>
+      <c r="AU78" s="13"/>
+      <c r="AV78" s="13"/>
+      <c r="AW78" s="13"/>
+      <c r="AX78" s="13"/>
+      <c r="AY78" s="13"/>
+      <c r="AZ78" s="13"/>
+      <c r="BA78" s="13"/>
+    </row>
+    <row r="79" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AQ79" s="13"/>
+      <c r="AR79" s="13"/>
+      <c r="AS79" s="13"/>
+      <c r="AT79" s="13"/>
+      <c r="AU79" s="13"/>
+      <c r="AV79" s="13"/>
+      <c r="AW79" s="13"/>
+      <c r="AX79" s="13"/>
+      <c r="AY79" s="13"/>
+      <c r="AZ79" s="13"/>
+      <c r="BA79" s="13"/>
+    </row>
+    <row r="80" spans="42:53" x14ac:dyDescent="0.2">
+      <c r="AR80" s="13"/>
+      <c r="AS80" s="13"/>
+    </row>
+    <row r="81" spans="44:45" x14ac:dyDescent="0.2">
+      <c r="AR81" s="13"/>
+      <c r="AS81" s="13"/>
+    </row>
+    <row r="82" spans="44:45" x14ac:dyDescent="0.2">
+      <c r="AR82" s="13"/>
+      <c r="AS82" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="X23:AB23"/>
-    <mergeCell ref="X30:AB30"/>
-    <mergeCell ref="D37:H37"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="R9:V9"/>
-    <mergeCell ref="R16:V16"/>
-    <mergeCell ref="J30:N30"/>
-    <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D9:H9"/>
-    <mergeCell ref="D16:H16"/>
-    <mergeCell ref="D23:H23"/>
-    <mergeCell ref="D30:H30"/>
-    <mergeCell ref="J23:N23"/>
-    <mergeCell ref="R37:V37"/>
-    <mergeCell ref="R23:V23"/>
-    <mergeCell ref="R30:V30"/>
+  <mergeCells count="26">
+    <mergeCell ref="Y4:AI4"/>
+    <mergeCell ref="X26:AB26"/>
+    <mergeCell ref="R12:V12"/>
+    <mergeCell ref="R19:V19"/>
+    <mergeCell ref="R26:V26"/>
+    <mergeCell ref="R40:V40"/>
+    <mergeCell ref="X33:AB33"/>
+    <mergeCell ref="R33:V33"/>
+    <mergeCell ref="AP21:AQ21"/>
+    <mergeCell ref="AP13:AQ13"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AP3:AZ3"/>
+    <mergeCell ref="AS37:AT37"/>
+    <mergeCell ref="AS29:AT29"/>
+    <mergeCell ref="AP37:AQ37"/>
+    <mergeCell ref="AP45:AQ45"/>
+    <mergeCell ref="AP29:AQ29"/>
+    <mergeCell ref="D39:H39"/>
+    <mergeCell ref="R5:V5"/>
+    <mergeCell ref="J32:N32"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="D11:H11"/>
+    <mergeCell ref="D18:H18"/>
+    <mergeCell ref="D25:H25"/>
+    <mergeCell ref="D32:H32"/>
+    <mergeCell ref="J25:N25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>